<commit_message>
21 maret 2023, sore sebelum pulang kantor
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478167C4-5C2C-419A-881D-61610947BD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0B682-5440-46C4-8680-02B47374A847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="216">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -950,6 +950,9 @@
   </si>
   <si>
     <t>2 - 3 November 2022</t>
+  </si>
+  <si>
+    <t>I.C.39</t>
   </si>
 </sst>
 </file>
@@ -1195,12 +1198,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1215,6 +1212,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1504,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1521,16 +1524,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
@@ -1749,25 +1752,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1775,13 +1778,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1813,16 +1816,16 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
@@ -1852,16 +1855,16 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
@@ -1918,16 +1921,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
@@ -2153,7 +2156,7 @@
         <v>87</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>72</v>
@@ -2227,16 +2230,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="26"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="7">
@@ -2395,16 +2398,16 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="26"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="24"/>
     </row>
     <row r="54" spans="1:8" ht="42.75">
       <c r="A54" s="7">
@@ -3934,16 +3937,16 @@
       <c r="V109" s="15"/>
     </row>
     <row r="110" spans="1:22" ht="15" customHeight="1">
-      <c r="A110" s="24" t="s">
+      <c r="A110" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="25"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="25"/>
-      <c r="G110" s="25"/>
-      <c r="H110" s="26"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="24"/>
     </row>
     <row r="111" spans="1:22">
       <c r="A111" s="7">
@@ -3958,16 +3961,16 @@
       <c r="H111" s="12"/>
     </row>
     <row r="112" spans="1:22">
-      <c r="A112" s="24" t="s">
+      <c r="A112" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="25"/>
-      <c r="H112" s="26"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="24"/>
     </row>
     <row r="113" spans="1:8" ht="57">
       <c r="A113" s="7">
@@ -3992,7 +3995,7 @@
         <v>1</v>
       </c>
       <c r="H113" s="16">
-        <f>F113*G113</f>
+        <f t="shared" ref="H113:H124" si="13">F113*G113</f>
         <v>1</v>
       </c>
     </row>
@@ -4019,7 +4022,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="16">
-        <f>F114*G114</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4046,7 +4049,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="16">
-        <f>F115*G115</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4073,7 +4076,7 @@
         <v>1</v>
       </c>
       <c r="H116" s="16">
-        <f>F116*G116</f>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4100,7 +4103,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="16">
-        <f>F117*G117</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4127,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="16">
-        <f>F118*G118</f>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4154,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="H119" s="16">
-        <f>F119*G119</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4181,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="16">
-        <f>F120*G120</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4208,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="16">
-        <f>F121*G121</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
@@ -4235,7 +4238,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="16">
-        <f>F122*G122</f>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4262,7 +4265,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="16">
-        <f>F123*G123</f>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
@@ -4289,20 +4292,20 @@
         <v>1</v>
       </c>
       <c r="H124" s="16">
-        <f>F124*G124</f>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="125" spans="1:8">
-      <c r="A125" s="21" t="s">
+      <c r="A125" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B125" s="21"/>
-      <c r="C125" s="21"/>
-      <c r="D125" s="21"/>
-      <c r="E125" s="21"/>
-      <c r="F125" s="21"/>
-      <c r="G125" s="21"/>
+      <c r="B125" s="26"/>
+      <c r="C125" s="26"/>
+      <c r="D125" s="26"/>
+      <c r="E125" s="26"/>
+      <c r="F125" s="26"/>
+      <c r="G125" s="26"/>
       <c r="H125" s="6">
         <f>SUM(H23:H124)</f>
         <v>73.484999999999943</v>
@@ -4326,11 +4329,11 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="22" t="s">
+      <c r="F127" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="G127" s="22"/>
-      <c r="H127" s="22"/>
+      <c r="G127" s="20"/>
+      <c r="H127" s="20"/>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" s="1"/>
@@ -4338,11 +4341,11 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="22" t="s">
+      <c r="F128" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G128" s="22"/>
-      <c r="H128" s="22"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="1"/>
@@ -4390,11 +4393,11 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="22" t="s">
+      <c r="F133" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G133" s="22"/>
-      <c r="H133" s="22"/>
+      <c r="G133" s="20"/>
+      <c r="H133" s="20"/>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" s="1"/>
@@ -4402,11 +4405,11 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="22" t="s">
+      <c r="F134" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G134" s="22"/>
-      <c r="H134" s="22"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="20"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="1"/>
@@ -4680,12 +4683,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A110:H110"/>
-    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A125:G125"/>
     <mergeCell ref="F127:H127"/>
@@ -4701,6 +4698,12 @@
     <mergeCell ref="A112:H112"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A105:H105"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A110:H110"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
23 maret jam 5 sore
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0B682-5440-46C4-8680-02B47374A847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E38A78-2952-473D-809C-9B95B1E2B417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="215">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -801,30 +801,6 @@
   </si>
   <si>
     <t>Membuat Program Aplikasi Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Menyusun Definisi </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Rule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Validasi Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
-    </r>
   </si>
   <si>
     <t>Menyusun Petunjuk Operasional Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
@@ -1198,6 +1174,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1212,12 +1194,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1505,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V161"/>
+  <dimension ref="A1:V160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,16 +1500,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
@@ -1752,25 +1728,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1778,13 +1754,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1816,16 +1792,16 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
@@ -1855,16 +1831,16 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
@@ -1921,16 +1897,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
@@ -2156,7 +2132,7 @@
         <v>87</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>72</v>
@@ -2230,16 +2206,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="7">
@@ -2398,16 +2374,16 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="24"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="26"/>
     </row>
     <row r="54" spans="1:8" ht="42.75">
       <c r="A54" s="7">
@@ -3517,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="H95" s="12">
-        <f t="shared" ref="H95:H104" si="12">F95*G95</f>
+        <f t="shared" ref="H95:H103" si="12">F95*G95</f>
         <v>0.88</v>
       </c>
     </row>
@@ -3704,59 +3680,75 @@
         <v>179</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D103" s="13"/>
       <c r="E103" s="9" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F103" s="10">
-        <v>0.44</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G103" s="11">
         <v>1</v>
       </c>
       <c r="H103" s="12">
         <f t="shared" si="12"/>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="104" spans="1:22" ht="42.75">
-      <c r="A104" s="7">
-        <v>51</v>
-      </c>
-      <c r="B104" s="8" t="s">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" ht="14.25" customHeight="1">
+      <c r="A104" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="C104" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D104" s="13"/>
-      <c r="E104" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F104" s="10">
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="15"/>
+      <c r="O104" s="15"/>
+      <c r="P104" s="15"/>
+      <c r="Q104" s="15"/>
+      <c r="R104" s="15"/>
+      <c r="S104" s="15"/>
+      <c r="T104" s="15"/>
+      <c r="U104" s="15"/>
+      <c r="V104" s="15"/>
+    </row>
+    <row r="105" spans="1:22" ht="35.25" customHeight="1">
+      <c r="A105" s="16">
+        <v>1</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D105" s="16">
+        <v>2021</v>
+      </c>
+      <c r="E105" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F105" s="16">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G104" s="11">
-        <v>1</v>
-      </c>
-      <c r="H104" s="12">
-        <f t="shared" si="12"/>
-        <v>0.16500000000000001</v>
-      </c>
-    </row>
-    <row r="105" spans="1:22" ht="14.25" customHeight="1">
-      <c r="A105" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="B105" s="28"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28"/>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="29"/>
+      <c r="G105" s="16">
+        <v>18</v>
+      </c>
+      <c r="H105" s="16">
+        <f>F105*G105</f>
+        <v>2.97</v>
+      </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
       <c r="K105" s="15"/>
@@ -3774,13 +3766,13 @@
     </row>
     <row r="106" spans="1:22" ht="35.25" customHeight="1">
       <c r="A106" s="16">
-        <v>1</v>
-      </c>
-      <c r="B106" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="18" t="s">
         <v>183</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D106" s="16">
         <v>2021</v>
@@ -3789,14 +3781,14 @@
         <v>36</v>
       </c>
       <c r="F106" s="16">
-        <v>0.16500000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="G106" s="16">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="H106" s="16">
         <f>F106*G106</f>
-        <v>2.97</v>
+        <v>4.16</v>
       </c>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
@@ -3815,29 +3807,29 @@
     </row>
     <row r="107" spans="1:22" ht="35.25" customHeight="1">
       <c r="A107" s="16">
-        <v>2</v>
-      </c>
-      <c r="B107" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C107" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C107" s="19" t="s">
-        <v>182</v>
-      </c>
       <c r="D107" s="16">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E107" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F107" s="16">
-        <v>0.08</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G107" s="16">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="H107" s="16">
         <f>F107*G107</f>
-        <v>4.16</v>
+        <v>2.97</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
@@ -3856,13 +3848,13 @@
     </row>
     <row r="108" spans="1:22" ht="35.25" customHeight="1">
       <c r="A108" s="16">
-        <v>3</v>
-      </c>
-      <c r="B108" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" s="18" t="s">
         <v>183</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D108" s="16">
         <v>2022</v>
@@ -3871,14 +3863,14 @@
         <v>36</v>
       </c>
       <c r="F108" s="16">
-        <v>0.16500000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="G108" s="16">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="H108" s="16">
         <f>F108*G108</f>
-        <v>2.97</v>
+        <v>4.16</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
@@ -3895,98 +3887,84 @@
       <c r="U108" s="15"/>
       <c r="V108" s="15"/>
     </row>
-    <row r="109" spans="1:22" ht="35.25" customHeight="1">
-      <c r="A109" s="16">
-        <v>4</v>
-      </c>
-      <c r="B109" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D109" s="16">
-        <v>2022</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F109" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="G109" s="16">
-        <v>52</v>
-      </c>
-      <c r="H109" s="16">
-        <f>F109*G109</f>
-        <v>4.16</v>
-      </c>
-      <c r="I109" s="15"/>
-      <c r="J109" s="15"/>
-      <c r="K109" s="15"/>
-      <c r="L109" s="15"/>
-      <c r="M109" s="15"/>
-      <c r="N109" s="15"/>
-      <c r="O109" s="15"/>
-      <c r="P109" s="15"/>
-      <c r="Q109" s="15"/>
-      <c r="R109" s="15"/>
-      <c r="S109" s="15"/>
-      <c r="T109" s="15"/>
-      <c r="U109" s="15"/>
-      <c r="V109" s="15"/>
-    </row>
-    <row r="110" spans="1:22" ht="15" customHeight="1">
-      <c r="A110" s="22" t="s">
+    <row r="109" spans="1:22" ht="15" customHeight="1">
+      <c r="A109" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="23"/>
-      <c r="C110" s="23"/>
-      <c r="D110" s="23"/>
-      <c r="E110" s="23"/>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
-      <c r="H110" s="24"/>
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="25"/>
+      <c r="H109" s="26"/>
+    </row>
+    <row r="110" spans="1:22">
+      <c r="A110" s="7">
+        <v>1</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="12"/>
     </row>
     <row r="111" spans="1:22">
-      <c r="A111" s="7">
-        <v>1</v>
-      </c>
-      <c r="B111" s="8"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="10"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="12"/>
-    </row>
-    <row r="112" spans="1:22">
-      <c r="A112" s="22" t="s">
+      <c r="A111" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B112" s="23"/>
-      <c r="C112" s="23"/>
-      <c r="D112" s="23"/>
-      <c r="E112" s="23"/>
-      <c r="F112" s="23"/>
-      <c r="G112" s="23"/>
-      <c r="H112" s="24"/>
-    </row>
-    <row r="113" spans="1:8" ht="57">
+      <c r="B111" s="25"/>
+      <c r="C111" s="25"/>
+      <c r="D111" s="25"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="25"/>
+      <c r="H111" s="26"/>
+    </row>
+    <row r="112" spans="1:22" ht="57">
+      <c r="A112" s="7">
+        <v>1</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D112" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F112" s="10">
+        <v>1</v>
+      </c>
+      <c r="G112" s="11">
+        <v>1</v>
+      </c>
+      <c r="H112" s="16">
+        <f t="shared" ref="H112:H123" si="13">F112*G112</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="42.75">
       <c r="A113" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C113" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D113" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="D113" s="13" t="s">
-        <v>193</v>
-      </c>
       <c r="E113" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F113" s="10">
         <v>1</v>
@@ -3995,25 +3973,25 @@
         <v>1</v>
       </c>
       <c r="H113" s="16">
-        <f t="shared" ref="H113:H124" si="13">F113*G113</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="42.75">
       <c r="A114" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>189</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D114" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E114" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="F114" s="10">
         <v>1</v>
@@ -4026,36 +4004,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="42.75">
+    <row r="115" spans="1:8" ht="57">
       <c r="A115" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F115" s="10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G115" s="11">
         <v>1</v>
       </c>
       <c r="H115" s="16">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="42.75">
       <c r="A116" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>196</v>
@@ -4067,88 +4045,88 @@
         <v>198</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F116" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G116" s="11">
         <v>1</v>
       </c>
       <c r="H116" s="16">
         <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="57">
+      <c r="A117" s="7">
+        <v>6</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D117" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F117" s="10">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="42.75">
-      <c r="A117" s="7">
-        <v>5</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D117" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F117" s="10">
-        <v>1</v>
       </c>
       <c r="G117" s="11">
         <v>1</v>
       </c>
       <c r="H117" s="16">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="42.75">
       <c r="A118" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D118" s="13" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F118" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G118" s="11">
         <v>1</v>
       </c>
       <c r="H118" s="16">
         <f t="shared" si="13"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="42.75">
       <c r="A119" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F119" s="10">
         <v>1</v>
@@ -4161,21 +4139,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="42.75">
+    <row r="120" spans="1:8" ht="57">
       <c r="A120" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D120" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F120" s="10">
         <v>1</v>
@@ -4190,46 +4168,46 @@
     </row>
     <row r="121" spans="1:8" ht="57">
       <c r="A121" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F121" s="10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G121" s="11">
         <v>1</v>
       </c>
       <c r="H121" s="16">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="42.75">
       <c r="A122" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>209</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D122" s="13" t="s">
         <v>211</v>
       </c>
       <c r="E122" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F122" s="10">
         <v>0.5</v>
@@ -4242,21 +4220,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="42.75">
+    <row r="123" spans="1:8" ht="57">
       <c r="A123" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D123" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F123" s="10">
         <v>0.5</v>
@@ -4269,59 +4247,44 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="57">
-      <c r="A124" s="7">
-        <v>12</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D124" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F124" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="G124" s="11">
-        <v>1</v>
-      </c>
-      <c r="H124" s="16">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
+    <row r="124" spans="1:8">
+      <c r="A124" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" s="21"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="21"/>
+      <c r="H124" s="6">
+        <f>SUM(H23:H123)</f>
+        <v>73.044999999999945</v>
       </c>
     </row>
     <row r="125" spans="1:8">
-      <c r="A125" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B125" s="26"/>
-      <c r="C125" s="26"/>
-      <c r="D125" s="26"/>
-      <c r="E125" s="26"/>
-      <c r="F125" s="26"/>
-      <c r="G125" s="26"/>
-      <c r="H125" s="6">
-        <f>SUM(H23:H124)</f>
-        <v>73.484999999999943</v>
-      </c>
+      <c r="A125" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
     </row>
     <row r="126" spans="1:8">
-      <c r="A126" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
+      <c r="F126" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="G126" s="22"/>
+      <c r="H126" s="22"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="1"/>
@@ -4329,11 +4292,11 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="G127" s="20"/>
-      <c r="H127" s="20"/>
+      <c r="F127" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G127" s="22"/>
+      <c r="H127" s="22"/>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" s="1"/>
@@ -4341,11 +4304,9 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G128" s="20"/>
-      <c r="H128" s="20"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="1"/>
@@ -4383,9 +4344,11 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="1"/>
-      <c r="G132" s="1"/>
-      <c r="H132" s="1"/>
+      <c r="F132" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G132" s="22"/>
+      <c r="H132" s="22"/>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" s="1"/>
@@ -4393,11 +4356,11 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G133" s="20"/>
-      <c r="H133" s="20"/>
+      <c r="F133" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G133" s="22"/>
+      <c r="H133" s="22"/>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" s="1"/>
@@ -4405,11 +4368,9 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G134" s="20"/>
-      <c r="H134" s="20"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="1"/>
@@ -4671,21 +4632,17 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:8">
-      <c r="A161" s="1"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="1"/>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
-      <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
-      <c r="H161" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A125:G125"/>
-    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="F126:H126"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -4695,15 +4652,9 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="A111:H111"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A105:H105"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A110:H110"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A104:H104"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
24 maret sebelum pulang kantor
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E38A78-2952-473D-809C-9B95B1E2B417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FE585C-6335-40E9-AB6B-5898F298363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="218">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Sub Unsur IVE. Pengembangan Kompetensi di Bidang Teknologi Informasi</t>
-  </si>
-  <si>
-    <t>Sub Unsur IIB. Manajemen Infrastruktur TI</t>
   </si>
   <si>
     <t>: Pembina Tingkat I/ IV / b</t>
@@ -929,6 +926,18 @@
   </si>
   <si>
     <t>I.C.39</t>
+  </si>
+  <si>
+    <t>Mengikuti Pelatihan "Pengolahan Susenas Maret 2021" sebagai Peserta Selama 8 Jam</t>
+  </si>
+  <si>
+    <t>Februari - September 2022</t>
+  </si>
+  <si>
+    <t>Februari -Desember 2022</t>
+  </si>
+  <si>
+    <t>Januari - Juli 2021</t>
   </si>
 </sst>
 </file>
@@ -1174,12 +1183,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,6 +1197,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1481,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V160"/>
+  <dimension ref="A1:V147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1500,16 +1509,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
@@ -1549,7 +1558,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1563,7 +1572,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1577,7 +1586,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1591,7 +1600,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1605,7 +1614,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1641,7 +1650,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1655,7 +1664,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1669,7 +1678,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1683,7 +1692,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1697,7 +1706,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1728,25 +1737,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1754,13 +1763,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1792,29 +1801,29 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
+      <c r="A22" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
         <v>1</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>28</v>
@@ -1831,32 +1840,32 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
+      <c r="A24" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
         <v>1</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="10">
         <v>0.33</v>
@@ -1874,16 +1883,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="E26" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" s="10">
         <v>0.15</v>
@@ -1897,32 +1906,32 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
         <v>1</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="10">
         <v>0.11</v>
@@ -1940,16 +1949,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" s="10">
         <v>0.11</v>
@@ -1967,13 +1976,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>28</v>
@@ -1994,13 +2003,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>28</v>
@@ -2021,16 +2030,16 @@
         <v>5</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="E32" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="10">
         <v>0.12</v>
@@ -2048,16 +2057,16 @@
         <v>6</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="F33" s="10">
         <v>0.12</v>
@@ -2075,16 +2084,16 @@
         <v>7</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F34" s="10">
         <v>0.12</v>
@@ -2102,16 +2111,16 @@
         <v>8</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F35" s="10">
         <v>0.12</v>
@@ -2129,16 +2138,16 @@
         <v>9</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D36" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="F36" s="10">
         <v>0.02</v>
@@ -2156,16 +2165,16 @@
         <v>10</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="E37" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="F37" s="10">
         <v>0.6</v>
@@ -2183,16 +2192,16 @@
         <v>11</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>80</v>
-      </c>
       <c r="E38" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" s="10">
         <v>0.01</v>
@@ -2206,720 +2215,930 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A39" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="26"/>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="A39" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24"/>
+    </row>
+    <row r="40" spans="1:8" ht="42.75">
       <c r="A40" s="7">
         <v>1</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="B40" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1</v>
+      </c>
+      <c r="H40" s="12">
+        <f t="shared" ref="H40:H80" si="9">F40*G40</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="42.75">
       <c r="A41" s="7">
         <v>2</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="B41" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="G41" s="11">
+        <v>1</v>
+      </c>
+      <c r="H41" s="12">
+        <f t="shared" si="9"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="42.75">
       <c r="A42" s="7">
         <v>3</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="12"/>
+      <c r="B42" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12">
+        <f t="shared" si="9"/>
+        <v>0.22</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="7">
         <v>4</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="12"/>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="B43" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="G43" s="11">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12">
+        <f t="shared" si="9"/>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="42.75">
       <c r="A44" s="7">
         <v>5</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="B44" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12">
+        <f t="shared" si="9"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="42.75">
       <c r="A45" s="7">
         <v>6</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="B45" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G45" s="11">
+        <v>1</v>
+      </c>
+      <c r="H45" s="12">
+        <f t="shared" si="9"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="42.75">
       <c r="A46" s="7">
         <v>7</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="12"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="B46" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12">
+        <f t="shared" si="9"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="42.75">
       <c r="A47" s="7">
         <v>8</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="12"/>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="B47" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G47" s="11">
+        <v>1</v>
+      </c>
+      <c r="H47" s="12">
+        <f t="shared" si="9"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="42.75">
       <c r="A48" s="7">
         <v>9</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="B48" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="G48" s="11">
+        <v>1</v>
+      </c>
+      <c r="H48" s="12">
+        <f t="shared" ref="H48:H57" si="10">F48*G48</f>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="42.75">
       <c r="A49" s="7">
         <v>10</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="B49" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F49" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="G49" s="11">
+        <v>1</v>
+      </c>
+      <c r="H49" s="12">
+        <f t="shared" si="10"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="42.75">
       <c r="A50" s="7">
         <v>11</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="7"/>
+      <c r="B50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="E50" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1</v>
+      </c>
+      <c r="H50" s="12">
+        <f t="shared" si="10"/>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="42.75">
       <c r="A51" s="7">
         <v>12</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="7"/>
+      <c r="B51" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="D51" s="13"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="12"/>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="E51" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="G51" s="11">
+        <v>1</v>
+      </c>
+      <c r="H51" s="12">
+        <f t="shared" si="10"/>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="42.75">
       <c r="A52" s="7">
         <v>13</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="7"/>
+      <c r="B52" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="D52" s="13"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="12"/>
-    </row>
-    <row r="53" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A53" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="26"/>
+      <c r="E52" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G52" s="11">
+        <v>1</v>
+      </c>
+      <c r="H52" s="12">
+        <f t="shared" si="10"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="42.75">
+      <c r="A53" s="7">
+        <v>14</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G53" s="11">
+        <v>1</v>
+      </c>
+      <c r="H53" s="12">
+        <f t="shared" si="10"/>
+        <v>0.44</v>
+      </c>
     </row>
     <row r="54" spans="1:8" ht="42.75">
       <c r="A54" s="7">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>89</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D54" s="13"/>
       <c r="E54" s="9" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="F54" s="10">
-        <v>0.88</v>
+        <v>1.21</v>
       </c>
       <c r="G54" s="11">
         <v>1</v>
       </c>
       <c r="H54" s="12">
-        <f t="shared" ref="H54:H94" si="9">F54*G54</f>
-        <v>0.88</v>
+        <f t="shared" si="10"/>
+        <v>1.21</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="42.75">
       <c r="A55" s="7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>89</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D55" s="13"/>
       <c r="E55" s="9" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="F55" s="10">
-        <v>0.88</v>
+        <v>1.21</v>
       </c>
       <c r="G55" s="11">
         <v>1</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" si="9"/>
-        <v>0.88</v>
+        <f t="shared" si="10"/>
+        <v>1.21</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="42.75">
       <c r="A56" s="7">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>89</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D56" s="13"/>
       <c r="E56" s="9" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="F56" s="10">
-        <v>0.22</v>
+        <v>0.44</v>
       </c>
       <c r="G56" s="11">
         <v>1</v>
       </c>
       <c r="H56" s="12">
-        <f t="shared" si="9"/>
-        <v>0.22</v>
+        <f t="shared" si="10"/>
+        <v>0.44</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="42.75">
       <c r="A57" s="7">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>89</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D57" s="13"/>
       <c r="E57" s="9" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="F57" s="10">
-        <v>0.22</v>
+        <v>0.44</v>
       </c>
       <c r="G57" s="11">
         <v>1</v>
       </c>
       <c r="H57" s="12">
-        <f t="shared" si="9"/>
-        <v>0.22</v>
+        <f t="shared" si="10"/>
+        <v>0.44</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="42.75">
       <c r="A58" s="7">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>94</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D58" s="13"/>
       <c r="E58" s="9" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="F58" s="10">
-        <v>0.44</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G58" s="11">
         <v>1</v>
       </c>
       <c r="H58" s="12">
-        <f t="shared" si="9"/>
-        <v>0.44</v>
+        <f t="shared" ref="H58:H59" si="11">F58*G58</f>
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="42.75">
       <c r="A59" s="7">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>95</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D59" s="13"/>
       <c r="E59" s="9" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="F59" s="10">
-        <v>0.44</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G59" s="11">
         <v>1</v>
       </c>
       <c r="H59" s="12">
-        <f t="shared" si="9"/>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="42.75">
+        <f t="shared" si="11"/>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="57">
       <c r="A60" s="7">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="F60" s="10">
-        <v>0.55000000000000004</v>
+        <v>0.11</v>
       </c>
       <c r="G60" s="11">
         <v>1</v>
       </c>
       <c r="H60" s="12">
         <f t="shared" si="9"/>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="42.75">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="57">
       <c r="A61" s="7">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="F61" s="10">
-        <v>0.55000000000000004</v>
+        <v>0.11</v>
       </c>
       <c r="G61" s="11">
         <v>1</v>
       </c>
       <c r="H61" s="12">
         <f t="shared" si="9"/>
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="42.75">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="57">
       <c r="A62" s="7">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F62" s="10">
-        <v>0.54</v>
+        <v>0.11</v>
       </c>
       <c r="G62" s="11">
         <v>1</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" ref="H62:H71" si="10">F62*G62</f>
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="57">
       <c r="A63" s="7">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F63" s="10">
-        <v>0.54</v>
+        <v>0.11</v>
       </c>
       <c r="G63" s="11">
         <v>1</v>
       </c>
       <c r="H63" s="12">
-        <f t="shared" si="10"/>
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="57">
       <c r="A64" s="7">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D64" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="E64" s="9" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F64" s="10">
-        <v>0.66</v>
+        <v>0.11</v>
       </c>
       <c r="G64" s="11">
         <v>1</v>
       </c>
       <c r="H64" s="12">
-        <f t="shared" si="10"/>
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="71.25">
       <c r="A65" s="7">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="E65" s="9" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F65" s="10">
-        <v>0.66</v>
+        <v>0.11</v>
       </c>
       <c r="G65" s="11">
         <v>1</v>
       </c>
       <c r="H65" s="12">
-        <f t="shared" si="10"/>
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="57">
       <c r="A66" s="7">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="E66" s="9" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F66" s="10">
-        <v>0.44</v>
+        <v>0.11</v>
       </c>
       <c r="G66" s="11">
         <v>1</v>
       </c>
       <c r="H66" s="12">
-        <f t="shared" si="10"/>
-        <v>0.44</v>
+        <f t="shared" si="9"/>
+        <v>0.11</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="42.75">
       <c r="A67" s="7">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D67" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>130</v>
+      </c>
       <c r="E67" s="9" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F67" s="10">
-        <v>0.44</v>
+        <v>0.11</v>
       </c>
       <c r="G67" s="11">
         <v>1</v>
       </c>
       <c r="H67" s="12">
-        <f t="shared" si="10"/>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="57">
       <c r="A68" s="7">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D68" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="E68" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F68" s="10">
-        <v>1.21</v>
+        <v>0.11</v>
       </c>
       <c r="G68" s="11">
         <v>1</v>
       </c>
       <c r="H68" s="12">
-        <f t="shared" si="10"/>
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="57">
       <c r="A69" s="7">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D69" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="E69" s="9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F69" s="10">
-        <v>1.21</v>
+        <v>0.11</v>
       </c>
       <c r="G69" s="11">
         <v>1</v>
       </c>
       <c r="H69" s="12">
-        <f t="shared" si="10"/>
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="57">
       <c r="A70" s="7">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D70" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>137</v>
+      </c>
       <c r="E70" s="9" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="F70" s="10">
-        <v>0.44</v>
+        <v>0.11</v>
       </c>
       <c r="G70" s="11">
         <v>1</v>
       </c>
       <c r="H70" s="12">
-        <f t="shared" si="10"/>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="57">
       <c r="A71" s="7">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D71" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="E71" s="9" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="F71" s="10">
-        <v>0.44</v>
+        <v>0.11</v>
       </c>
       <c r="G71" s="11">
         <v>1</v>
       </c>
       <c r="H71" s="12">
-        <f t="shared" si="10"/>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="57">
       <c r="A72" s="7">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="E72" s="9" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="F72" s="10">
-        <v>0.16500000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="G72" s="11">
         <v>1</v>
       </c>
       <c r="H72" s="12">
-        <f t="shared" ref="H72:H73" si="11">F72*G72</f>
-        <v>0.16500000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="42.75">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="57">
       <c r="A73" s="7">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D73" s="13"/>
+        <v>117</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="E73" s="9" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="F73" s="10">
-        <v>0.16500000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="G73" s="11">
         <v>1</v>
       </c>
       <c r="H73" s="12">
-        <f t="shared" si="11"/>
-        <v>0.16500000000000001</v>
+        <f t="shared" si="9"/>
+        <v>0.11</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="57">
       <c r="A74" s="7">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B74" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D74" s="13" t="s">
+      <c r="D74" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="F74" s="10">
         <v>0.11</v>
@@ -2932,21 +3151,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="57">
+    <row r="75" spans="1:8" ht="71.25">
       <c r="A75" s="7">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F75" s="10">
         <v>0.11</v>
@@ -2961,19 +3180,19 @@
     </row>
     <row r="76" spans="1:8" ht="57">
       <c r="A76" s="7">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D76" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F76" s="10">
         <v>0.11</v>
@@ -2988,19 +3207,19 @@
     </row>
     <row r="77" spans="1:8" ht="57">
       <c r="A77" s="7">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F77" s="10">
         <v>0.11</v>
@@ -3013,21 +3232,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="57">
+    <row r="78" spans="1:8" ht="71.25">
       <c r="A78" s="7">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F78" s="10">
         <v>0.11</v>
@@ -3040,21 +3259,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="71.25">
+    <row r="79" spans="1:8" ht="57">
       <c r="A79" s="7">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F79" s="10">
         <v>0.11</v>
@@ -3069,19 +3288,19 @@
     </row>
     <row r="80" spans="1:8" ht="57">
       <c r="A80" s="7">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F80" s="10">
         <v>0.11</v>
@@ -3094,1178 +3313,965 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="42.75">
+    <row r="81" spans="1:22" ht="42.75">
       <c r="A81" s="7">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>131</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D81" s="13"/>
       <c r="E81" s="9" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="F81" s="10">
-        <v>0.11</v>
+        <v>0.88</v>
       </c>
       <c r="G81" s="11">
         <v>1</v>
       </c>
       <c r="H81" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="57">
+        <f t="shared" ref="H81:H89" si="12">F81*G81</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" ht="42.75">
       <c r="A82" s="7">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>135</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D82" s="13"/>
       <c r="E82" s="9" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="F82" s="10">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="G82" s="11">
         <v>1</v>
       </c>
       <c r="H82" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="57">
-      <c r="A83" s="7">
-        <v>30</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F83" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G83" s="11">
-        <v>1</v>
-      </c>
-      <c r="H83" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="57">
-      <c r="A84" s="7">
-        <v>31</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D84" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G84" s="11">
-        <v>1</v>
-      </c>
-      <c r="H84" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="57">
-      <c r="A85" s="7">
-        <v>32</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F85" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G85" s="11">
-        <v>1</v>
-      </c>
-      <c r="H85" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="57">
-      <c r="A86" s="7">
-        <v>33</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D86" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F86" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G86" s="11">
-        <v>1</v>
-      </c>
-      <c r="H86" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="57">
-      <c r="A87" s="7">
-        <v>34</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D87" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F87" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G87" s="11">
-        <v>1</v>
-      </c>
-      <c r="H87" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="57">
-      <c r="A88" s="7">
-        <v>35</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F88" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G88" s="11">
-        <v>1</v>
-      </c>
-      <c r="H88" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="71.25">
-      <c r="A89" s="7">
-        <v>36</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F89" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G89" s="11">
-        <v>1</v>
-      </c>
-      <c r="H89" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="57">
-      <c r="A90" s="7">
-        <v>37</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F90" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G90" s="11">
-        <v>1</v>
-      </c>
-      <c r="H90" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="57">
-      <c r="A91" s="7">
-        <v>38</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F91" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G91" s="11">
-        <v>1</v>
-      </c>
-      <c r="H91" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="71.25">
-      <c r="A92" s="7">
-        <v>39</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D92" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F92" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G92" s="11">
-        <v>1</v>
-      </c>
-      <c r="H92" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="57">
-      <c r="A93" s="7">
-        <v>40</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F93" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G93" s="11">
-        <v>1</v>
-      </c>
-      <c r="H93" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="57">
-      <c r="A94" s="7">
-        <v>41</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F94" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G94" s="11">
-        <v>1</v>
-      </c>
-      <c r="H94" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="42.75">
-      <c r="A95" s="7">
-        <v>42</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D95" s="13"/>
-      <c r="E95" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F95" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="G95" s="11">
-        <v>1</v>
-      </c>
-      <c r="H95" s="12">
-        <f t="shared" ref="H95:H103" si="12">F95*G95</f>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="42.75">
-      <c r="A96" s="7">
-        <v>43</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D96" s="13"/>
-      <c r="E96" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F96" s="10">
-        <v>0.22</v>
-      </c>
-      <c r="G96" s="11">
-        <v>1</v>
-      </c>
-      <c r="H96" s="12">
         <f t="shared" si="12"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="42.75">
-      <c r="A97" s="7">
+    <row r="83" spans="1:22" ht="42.75">
+      <c r="A83" s="7">
         <v>44</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D97" s="13"/>
-      <c r="E97" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F97" s="10">
+      <c r="B83" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D83" s="13"/>
+      <c r="E83" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="10">
         <v>0.44</v>
       </c>
-      <c r="G97" s="11">
-        <v>1</v>
-      </c>
-      <c r="H97" s="12">
+      <c r="G83" s="11">
+        <v>1</v>
+      </c>
+      <c r="H83" s="12">
         <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="42.75">
-      <c r="A98" s="7">
+    <row r="84" spans="1:22" ht="42.75">
+      <c r="A84" s="7">
         <v>45</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D98" s="13"/>
-      <c r="E98" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F98" s="10">
+      <c r="B84" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D84" s="13"/>
+      <c r="E84" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F84" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G98" s="11">
-        <v>1</v>
-      </c>
-      <c r="H98" s="12">
+      <c r="G84" s="11">
+        <v>1</v>
+      </c>
+      <c r="H84" s="12">
         <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="42.75">
-      <c r="A99" s="7">
+    <row r="85" spans="1:22" ht="42.75">
+      <c r="A85" s="7">
         <v>46</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C99" s="7" t="s">
+      <c r="B85" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D85" s="13"/>
+      <c r="E85" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D99" s="13"/>
-      <c r="E99" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F99" s="10">
+      <c r="F85" s="10">
         <v>0.54</v>
       </c>
-      <c r="G99" s="11">
-        <v>1</v>
-      </c>
-      <c r="H99" s="12">
+      <c r="G85" s="11">
+        <v>1</v>
+      </c>
+      <c r="H85" s="12">
         <f t="shared" si="12"/>
         <v>0.54</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="42.75">
-      <c r="A100" s="7">
+    <row r="86" spans="1:22" ht="42.75">
+      <c r="A86" s="7">
         <v>47</v>
       </c>
-      <c r="B100" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C100" s="7" t="s">
+      <c r="B86" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" s="13"/>
+      <c r="E86" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D100" s="13"/>
-      <c r="E100" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F100" s="10">
+      <c r="F86" s="10">
         <v>0.66</v>
       </c>
-      <c r="G100" s="11">
-        <v>1</v>
-      </c>
-      <c r="H100" s="12">
+      <c r="G86" s="11">
+        <v>1</v>
+      </c>
+      <c r="H86" s="12">
         <f t="shared" si="12"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="42.75">
-      <c r="A101" s="7">
+    <row r="87" spans="1:22" ht="42.75">
+      <c r="A87" s="7">
         <v>48</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C101" s="7" t="s">
+      <c r="B87" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D87" s="13"/>
+      <c r="E87" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D101" s="13"/>
-      <c r="E101" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F101" s="10">
+      <c r="F87" s="10">
         <v>0.44</v>
       </c>
-      <c r="G101" s="11">
-        <v>1</v>
-      </c>
-      <c r="H101" s="12">
+      <c r="G87" s="11">
+        <v>1</v>
+      </c>
+      <c r="H87" s="12">
         <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="42.75">
-      <c r="A102" s="7">
+    <row r="88" spans="1:22" ht="42.75">
+      <c r="A88" s="7">
         <v>49</v>
       </c>
-      <c r="B102" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C102" s="7" t="s">
+      <c r="B88" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" s="13"/>
+      <c r="E88" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D102" s="13"/>
-      <c r="E102" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F102" s="10">
+      <c r="F88" s="10">
         <v>1.21</v>
       </c>
-      <c r="G102" s="11">
-        <v>1</v>
-      </c>
-      <c r="H102" s="12">
+      <c r="G88" s="11">
+        <v>1</v>
+      </c>
+      <c r="H88" s="12">
         <f t="shared" si="12"/>
         <v>1.21</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="42.75">
-      <c r="A103" s="7">
+    <row r="89" spans="1:22" ht="42.75">
+      <c r="A89" s="7">
         <v>50</v>
       </c>
-      <c r="B103" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C103" s="7" t="s">
+      <c r="B89" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" s="13"/>
+      <c r="E89" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D103" s="13"/>
-      <c r="E103" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="F103" s="10">
+      <c r="F89" s="10">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G103" s="11">
-        <v>1</v>
-      </c>
-      <c r="H103" s="12">
+      <c r="G89" s="11">
+        <v>1</v>
+      </c>
+      <c r="H89" s="12">
         <f t="shared" si="12"/>
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="14.25" customHeight="1">
-      <c r="A104" s="27" t="s">
+    <row r="90" spans="1:22" ht="14.25" customHeight="1">
+      <c r="A90" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="15"/>
+      <c r="N90" s="15"/>
+      <c r="O90" s="15"/>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="15"/>
+      <c r="R90" s="15"/>
+      <c r="S90" s="15"/>
+      <c r="T90" s="15"/>
+      <c r="U90" s="15"/>
+      <c r="V90" s="15"/>
+    </row>
+    <row r="91" spans="1:22" ht="28.5">
+      <c r="A91" s="16">
+        <v>1</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E91" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F91" s="16">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G91" s="16">
+        <v>18</v>
+      </c>
+      <c r="H91" s="16">
+        <f>F91*G91</f>
+        <v>2.97</v>
+      </c>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="15"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+      <c r="R91" s="15"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="15"/>
+      <c r="U91" s="15"/>
+      <c r="V91" s="15"/>
+    </row>
+    <row r="92" spans="1:22" ht="42.75">
+      <c r="A92" s="16">
+        <v>2</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="B104" s="28"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="29"/>
-      <c r="I104" s="15"/>
-      <c r="J104" s="15"/>
-      <c r="K104" s="15"/>
-      <c r="L104" s="15"/>
-      <c r="M104" s="15"/>
-      <c r="N104" s="15"/>
-      <c r="O104" s="15"/>
-      <c r="P104" s="15"/>
-      <c r="Q104" s="15"/>
-      <c r="R104" s="15"/>
-      <c r="S104" s="15"/>
-      <c r="T104" s="15"/>
-      <c r="U104" s="15"/>
-      <c r="V104" s="15"/>
-    </row>
-    <row r="105" spans="1:22" ht="35.25" customHeight="1">
-      <c r="A105" s="16">
-        <v>1</v>
-      </c>
-      <c r="B105" s="17" t="s">
+      <c r="D92" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E92" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F92" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="G92" s="16">
+        <v>52</v>
+      </c>
+      <c r="H92" s="16">
+        <f>F92*G92</f>
+        <v>4.16</v>
+      </c>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="15"/>
+      <c r="O92" s="15"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+      <c r="R92" s="15"/>
+      <c r="S92" s="15"/>
+      <c r="T92" s="15"/>
+      <c r="U92" s="15"/>
+      <c r="V92" s="15"/>
+    </row>
+    <row r="93" spans="1:22" ht="42.75">
+      <c r="A93" s="16">
+        <v>3</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E93" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F93" s="16">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G93" s="16">
+        <v>18</v>
+      </c>
+      <c r="H93" s="16">
+        <f>F93*G93</f>
+        <v>2.97</v>
+      </c>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="15"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="15"/>
+      <c r="Q93" s="15"/>
+      <c r="R93" s="15"/>
+      <c r="S93" s="15"/>
+      <c r="T93" s="15"/>
+      <c r="U93" s="15"/>
+      <c r="V93" s="15"/>
+    </row>
+    <row r="94" spans="1:22" ht="42.75">
+      <c r="A94" s="16">
+        <v>4</v>
+      </c>
+      <c r="B94" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C94" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="E94" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F94" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="G94" s="16">
+        <v>52</v>
+      </c>
+      <c r="H94" s="16">
+        <f>F94*G94</f>
+        <v>4.16</v>
+      </c>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="15"/>
+      <c r="R94" s="15"/>
+      <c r="S94" s="15"/>
+      <c r="T94" s="15"/>
+      <c r="U94" s="15"/>
+      <c r="V94" s="15"/>
+    </row>
+    <row r="95" spans="1:22" ht="15" customHeight="1">
+      <c r="A95" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="24"/>
+    </row>
+    <row r="96" spans="1:22">
+      <c r="A96" s="7">
+        <v>1</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="12"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="24"/>
+    </row>
+    <row r="98" spans="1:8" ht="57">
+      <c r="A98" s="7">
+        <v>1</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D105" s="16">
-        <v>2021</v>
-      </c>
-      <c r="E105" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F105" s="16">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G105" s="16">
-        <v>18</v>
-      </c>
-      <c r="H105" s="16">
-        <f>F105*G105</f>
-        <v>2.97</v>
-      </c>
-      <c r="I105" s="15"/>
-      <c r="J105" s="15"/>
-      <c r="K105" s="15"/>
-      <c r="L105" s="15"/>
-      <c r="M105" s="15"/>
-      <c r="N105" s="15"/>
-      <c r="O105" s="15"/>
-      <c r="P105" s="15"/>
-      <c r="Q105" s="15"/>
-      <c r="R105" s="15"/>
-      <c r="S105" s="15"/>
-      <c r="T105" s="15"/>
-      <c r="U105" s="15"/>
-      <c r="V105" s="15"/>
-    </row>
-    <row r="106" spans="1:22" ht="35.25" customHeight="1">
-      <c r="A106" s="16">
+      <c r="D98" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F98" s="10">
+        <v>1</v>
+      </c>
+      <c r="G98" s="11">
+        <v>1</v>
+      </c>
+      <c r="H98" s="16">
+        <f t="shared" ref="H98:H110" si="13">F98*G98</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="42.75">
+      <c r="A99" s="7">
         <v>2</v>
       </c>
-      <c r="B106" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C106" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D106" s="16">
-        <v>2021</v>
-      </c>
-      <c r="E106" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F106" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="G106" s="16">
-        <v>52</v>
-      </c>
-      <c r="H106" s="16">
-        <f>F106*G106</f>
-        <v>4.16</v>
-      </c>
-      <c r="I106" s="15"/>
-      <c r="J106" s="15"/>
-      <c r="K106" s="15"/>
-      <c r="L106" s="15"/>
-      <c r="M106" s="15"/>
-      <c r="N106" s="15"/>
-      <c r="O106" s="15"/>
-      <c r="P106" s="15"/>
-      <c r="Q106" s="15"/>
-      <c r="R106" s="15"/>
-      <c r="S106" s="15"/>
-      <c r="T106" s="15"/>
-      <c r="U106" s="15"/>
-      <c r="V106" s="15"/>
-    </row>
-    <row r="107" spans="1:22" ht="35.25" customHeight="1">
-      <c r="A107" s="16">
+      <c r="B99" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F99" s="10">
+        <v>1</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1</v>
+      </c>
+      <c r="H99" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="42.75">
+      <c r="A100" s="7">
         <v>3</v>
       </c>
-      <c r="B107" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C107" s="19" t="s">
+      <c r="B100" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D107" s="16">
-        <v>2022</v>
-      </c>
-      <c r="E107" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F107" s="16">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G107" s="16">
-        <v>18</v>
-      </c>
-      <c r="H107" s="16">
-        <f>F107*G107</f>
-        <v>2.97</v>
-      </c>
-      <c r="I107" s="15"/>
-      <c r="J107" s="15"/>
-      <c r="K107" s="15"/>
-      <c r="L107" s="15"/>
-      <c r="M107" s="15"/>
-      <c r="N107" s="15"/>
-      <c r="O107" s="15"/>
-      <c r="P107" s="15"/>
-      <c r="Q107" s="15"/>
-      <c r="R107" s="15"/>
-      <c r="S107" s="15"/>
-      <c r="T107" s="15"/>
-      <c r="U107" s="15"/>
-      <c r="V107" s="15"/>
-    </row>
-    <row r="108" spans="1:22" ht="35.25" customHeight="1">
-      <c r="A108" s="16">
+      <c r="D100" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F100" s="10">
+        <v>1</v>
+      </c>
+      <c r="G100" s="11">
+        <v>1</v>
+      </c>
+      <c r="H100" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="42.75">
+      <c r="A101" s="7">
         <v>4</v>
       </c>
-      <c r="B108" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D108" s="16">
-        <v>2022</v>
-      </c>
-      <c r="E108" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F108" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="G108" s="16">
-        <v>52</v>
-      </c>
-      <c r="H108" s="16">
-        <f>F108*G108</f>
-        <v>4.16</v>
-      </c>
-      <c r="I108" s="15"/>
-      <c r="J108" s="15"/>
-      <c r="K108" s="15"/>
-      <c r="L108" s="15"/>
-      <c r="M108" s="15"/>
-      <c r="N108" s="15"/>
-      <c r="O108" s="15"/>
-      <c r="P108" s="15"/>
-      <c r="Q108" s="15"/>
-      <c r="R108" s="15"/>
-      <c r="S108" s="15"/>
-      <c r="T108" s="15"/>
-      <c r="U108" s="15"/>
-      <c r="V108" s="15"/>
-    </row>
-    <row r="109" spans="1:22" ht="15" customHeight="1">
-      <c r="A109" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
-      <c r="H109" s="26"/>
-    </row>
-    <row r="110" spans="1:22">
-      <c r="A110" s="7">
-        <v>1</v>
-      </c>
-      <c r="B110" s="8"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="10"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="12"/>
-    </row>
-    <row r="111" spans="1:22">
-      <c r="A111" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B111" s="25"/>
-      <c r="C111" s="25"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="25"/>
-      <c r="G111" s="25"/>
-      <c r="H111" s="26"/>
-    </row>
-    <row r="112" spans="1:22" ht="57">
-      <c r="A112" s="7">
-        <v>1</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D112" s="13" t="s">
+      <c r="B101" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C101" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E112" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F112" s="10">
-        <v>1</v>
-      </c>
-      <c r="G112" s="11">
-        <v>1</v>
-      </c>
-      <c r="H112" s="16">
-        <f t="shared" ref="H112:H123" si="13">F112*G112</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="42.75">
-      <c r="A113" s="7">
-        <v>2</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C113" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D113" s="13" t="s">
+      <c r="D101" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E101" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="E113" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F113" s="10">
-        <v>1</v>
-      </c>
-      <c r="G113" s="11">
-        <v>1</v>
-      </c>
-      <c r="H113" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="42.75">
-      <c r="A114" s="7">
-        <v>3</v>
-      </c>
-      <c r="B114" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D114" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F114" s="10">
-        <v>1</v>
-      </c>
-      <c r="G114" s="11">
-        <v>1</v>
-      </c>
-      <c r="H114" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="57">
-      <c r="A115" s="7">
-        <v>4</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D115" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F115" s="10">
+      <c r="F101" s="10">
         <v>0.5</v>
       </c>
-      <c r="G115" s="11">
-        <v>1</v>
-      </c>
-      <c r="H115" s="16">
+      <c r="G101" s="11">
+        <v>1</v>
+      </c>
+      <c r="H101" s="16">
+        <f t="shared" ref="H101" si="14">F101*G101</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="57">
+      <c r="A102" s="7">
+        <v>5</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F102" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G102" s="11">
+        <v>1</v>
+      </c>
+      <c r="H102" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="42.75">
-      <c r="A116" s="7">
-        <v>5</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D116" s="13" t="s">
+    <row r="103" spans="1:8" ht="42.75">
+      <c r="A103" s="7">
+        <v>6</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F103" s="10">
+        <v>1</v>
+      </c>
+      <c r="G103" s="11">
+        <v>1</v>
+      </c>
+      <c r="H103" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="57">
+      <c r="A104" s="7">
+        <v>7</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E116" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F116" s="10">
-        <v>1</v>
-      </c>
-      <c r="G116" s="11">
-        <v>1</v>
-      </c>
-      <c r="H116" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="57">
-      <c r="A117" s="7">
-        <v>6</v>
-      </c>
-      <c r="B117" s="8" t="s">
+      <c r="C104" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D104" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C117" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D117" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F117" s="10">
+      <c r="E104" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F104" s="10">
         <v>0.5</v>
       </c>
-      <c r="G117" s="11">
-        <v>1</v>
-      </c>
-      <c r="H117" s="16">
+      <c r="G104" s="11">
+        <v>1</v>
+      </c>
+      <c r="H104" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="42.75">
-      <c r="A118" s="7">
-        <v>7</v>
-      </c>
-      <c r="B118" s="8" t="s">
+    <row r="105" spans="1:8" ht="42.75">
+      <c r="A105" s="7">
+        <v>8</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D105" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C118" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D118" s="13" t="s">
+      <c r="E105" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F105" s="10">
+        <v>1</v>
+      </c>
+      <c r="G105" s="11">
+        <v>1</v>
+      </c>
+      <c r="H105" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="42.75">
+      <c r="A106" s="7">
+        <v>9</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F106" s="10">
+        <v>1</v>
+      </c>
+      <c r="G106" s="11">
+        <v>1</v>
+      </c>
+      <c r="H106" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="57">
+      <c r="A107" s="7">
+        <v>10</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F107" s="10">
+        <v>1</v>
+      </c>
+      <c r="G107" s="11">
+        <v>1</v>
+      </c>
+      <c r="H107" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="57">
+      <c r="A108" s="7">
+        <v>11</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E118" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F118" s="10">
-        <v>1</v>
-      </c>
-      <c r="G118" s="11">
-        <v>1</v>
-      </c>
-      <c r="H118" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="42.75">
-      <c r="A119" s="7">
-        <v>8</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D119" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E119" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F119" s="10">
-        <v>1</v>
-      </c>
-      <c r="G119" s="11">
-        <v>1</v>
-      </c>
-      <c r="H119" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="57">
-      <c r="A120" s="7">
-        <v>9</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D120" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E120" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F120" s="10">
-        <v>1</v>
-      </c>
-      <c r="G120" s="11">
-        <v>1</v>
-      </c>
-      <c r="H120" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="57">
-      <c r="A121" s="7">
-        <v>10</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D121" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="E121" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F121" s="10">
+      <c r="C108" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F108" s="10">
         <v>0.5</v>
       </c>
-      <c r="G121" s="11">
-        <v>1</v>
-      </c>
-      <c r="H121" s="16">
+      <c r="G108" s="11">
+        <v>1</v>
+      </c>
+      <c r="H108" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="42.75">
-      <c r="A122" s="7">
-        <v>11</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D122" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F122" s="10">
+    <row r="109" spans="1:8" ht="42.75">
+      <c r="A109" s="7">
+        <v>12</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F109" s="10">
         <v>0.5</v>
       </c>
-      <c r="G122" s="11">
-        <v>1</v>
-      </c>
-      <c r="H122" s="16">
+      <c r="G109" s="11">
+        <v>1</v>
+      </c>
+      <c r="H109" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="57">
-      <c r="A123" s="7">
-        <v>12</v>
-      </c>
-      <c r="B123" s="8" t="s">
+    <row r="110" spans="1:8" ht="57">
+      <c r="A110" s="7">
+        <v>13</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D110" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C123" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D123" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E123" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F123" s="10">
+      <c r="E110" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F110" s="10">
         <v>0.5</v>
       </c>
-      <c r="G123" s="11">
-        <v>1</v>
-      </c>
-      <c r="H123" s="16">
+      <c r="G110" s="11">
+        <v>1</v>
+      </c>
+      <c r="H110" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="6">
+        <f>SUM(H23:H110)</f>
+        <v>73.544999999999945</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="1"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="1"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="1"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="1"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="1"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="1"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+    </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B124" s="21"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="21"/>
-      <c r="E124" s="21"/>
-      <c r="F124" s="21"/>
-      <c r="G124" s="21"/>
-      <c r="H124" s="6">
-        <f>SUM(H23:H123)</f>
-        <v>73.044999999999945</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
     </row>
     <row r="125" spans="1:8">
-      <c r="A125" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -4280,11 +4286,9 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="G126" s="22"/>
-      <c r="H126" s="22"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="1"/>
@@ -4292,11 +4296,9 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G127" s="22"/>
-      <c r="H127" s="22"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" s="1"/>
@@ -4344,11 +4346,9 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="G132" s="22"/>
-      <c r="H132" s="22"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" s="1"/>
@@ -4356,11 +4356,9 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G133" s="22"/>
-      <c r="H133" s="22"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" s="1"/>
@@ -4502,147 +4500,11 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:8">
-      <c r="A148" s="1"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
-      <c r="H148" s="1"/>
-    </row>
-    <row r="149" spans="1:8">
-      <c r="A149" s="1"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="1"/>
-      <c r="H149" s="1"/>
-    </row>
-    <row r="150" spans="1:8">
-      <c r="A150" s="1"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1"/>
-    </row>
-    <row r="151" spans="1:8">
-      <c r="A151" s="1"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="F151" s="1"/>
-      <c r="G151" s="1"/>
-      <c r="H151" s="1"/>
-    </row>
-    <row r="152" spans="1:8">
-      <c r="A152" s="1"/>
-      <c r="B152" s="2"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-      <c r="G152" s="1"/>
-      <c r="H152" s="1"/>
-    </row>
-    <row r="153" spans="1:8">
-      <c r="A153" s="1"/>
-      <c r="B153" s="2"/>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
-      <c r="H153" s="1"/>
-    </row>
-    <row r="154" spans="1:8">
-      <c r="A154" s="1"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="1"/>
-      <c r="D154" s="1"/>
-      <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
-      <c r="G154" s="1"/>
-      <c r="H154" s="1"/>
-    </row>
-    <row r="155" spans="1:8">
-      <c r="A155" s="1"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="1"/>
-      <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
-      <c r="F155" s="1"/>
-      <c r="G155" s="1"/>
-      <c r="H155" s="1"/>
-    </row>
-    <row r="156" spans="1:8">
-      <c r="A156" s="1"/>
-      <c r="B156" s="2"/>
-      <c r="C156" s="1"/>
-      <c r="D156" s="1"/>
-      <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
-      <c r="H156" s="1"/>
-    </row>
-    <row r="157" spans="1:8">
-      <c r="A157" s="1"/>
-      <c r="B157" s="2"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="1"/>
-    </row>
-    <row r="158" spans="1:8">
-      <c r="A158" s="1"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="1"/>
-    </row>
-    <row r="159" spans="1:8">
-      <c r="A159" s="1"/>
-      <c r="B159" s="2"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
-      <c r="H159" s="1"/>
-    </row>
-    <row r="160" spans="1:8">
-      <c r="A160" s="1"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="1"/>
-      <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
-      <c r="F160" s="1"/>
-      <c r="G160" s="1"/>
-      <c r="H160" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="A22:H22"/>
+  <mergeCells count="20">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A124:G124"/>
-    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="A111:G111"/>
+    <mergeCell ref="F113:H113"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -4651,10 +4513,15 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A111:H111"/>
+    <mergeCell ref="A97:H97"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A104:H104"/>
+    <mergeCell ref="A90:H90"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
25 maret 2022, sabtu sebelum pulang
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FE585C-6335-40E9-AB6B-5898F298363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C75A804-6A7D-458A-98F2-98C16A72DCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="247">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -391,30 +391,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> SUSENAS Maret 2021 Pada Komputer Server di Pusat Pengolahan BPS Kabupaten Kuantan Singingi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Melakukan Instalasi dan konfigurasi </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>DBMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> SAKERNAS Agustus 2021 Pada Komputer Server di Pusat Pengolahan BPS Kabupaten Kuantan Singingi</t>
     </r>
   </si>
   <si>
@@ -938,6 +914,117 @@
   </si>
   <si>
     <t>Januari - Juli 2021</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Melakukan Instalasi dan Konfigurasi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>DBMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> SAKERNAS Agustus 2021 Pada Komputer Server di Pusat Pengolahan BPS Kabupaten Kuantan Singingi</t>
+    </r>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Updating SAKERNAS Februari 2022 (Versi P22Feb.1) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Updating SAKERNAS Februari 2022 (Versi P22Feb.2) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Sampel SAKERNAS Februari 2022 (Versi AK22Feb.1) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Sampel SAKERNAS Februari 2022 (Versi AK22Feb.2) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Server Entri Data Sampel SUSENAS Maret 2022 (Versi SERVER 1.0.0) Pada Komputer Server di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Client Entri Data Sampel SUSENAS Maret 2022 (Versi CLIENT 1.0) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Sampel SAKERNAS Agustus 2022 (Versi AK22Agt.1) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Sampel SAKERNAS Agustus 2022 (Versi AK22Agt.3) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Server Entri Data Sampel SUSENAS September 2022 (Versi SERVER 1.0.0) Pada Komputer Server di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Client Entri Data Sampel SUSENAS September 2022 (Versi CLIENT 1.0) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Instalasi Program Client Entri Data Sampel SUSENAS September 2022 (Versi CLIENT 2.0) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>30 Januari 2022</t>
+  </si>
+  <si>
+    <t>2 Februari 2022</t>
+  </si>
+  <si>
+    <t>10 Februari 2022</t>
+  </si>
+  <si>
+    <t>18 Februari 2022</t>
+  </si>
+  <si>
+    <t>1 April 2022</t>
+  </si>
+  <si>
+    <t>10 Agustus 2022</t>
+  </si>
+  <si>
+    <t>Instalasi Program Entri Data Sampel SAKERNAS Agustus 2022 (Versi AK22Agt.1 DB3) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>16 Agustus 2022</t>
+  </si>
+  <si>
+    <t>15 Agustus 2022</t>
+  </si>
+  <si>
+    <t>19 September 2022</t>
+  </si>
+  <si>
+    <t>4 Oktober 2022</t>
+  </si>
+  <si>
+    <t>Januari - Desember 2022</t>
+  </si>
+  <si>
+    <t>Membuat Peta Tematik Rinci Kegiatan Digitalisasi Titik Bangunan Hasil SP2020</t>
+  </si>
+  <si>
+    <t>III.C.2</t>
+  </si>
+  <si>
+    <t>1-15 Agustus 2021</t>
+  </si>
+  <si>
+    <t>Peta Tematik Rinci</t>
+  </si>
+  <si>
+    <t>Membuat Peta Tematik Rinci Kegiatan Pemutakhiran Kerangka Geospasial dan Muatan Wilkerstat ST2023</t>
+  </si>
+  <si>
+    <t>1-31 Oktober 2022</t>
   </si>
 </sst>
 </file>
@@ -1183,6 +1270,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1197,12 +1290,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1490,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V147"/>
+  <dimension ref="A1:V162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1509,16 +1596,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
@@ -1737,25 +1824,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1763,13 +1850,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1801,16 +1888,16 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
@@ -1840,16 +1927,16 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
@@ -1906,16 +1993,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
@@ -2084,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>84</v>
+        <v>217</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>65</v>
@@ -2111,7 +2198,7 @@
         <v>8</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>65</v>
@@ -2138,10 +2225,10 @@
         <v>9</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>71</v>
@@ -2210,611 +2297,611 @@
         <v>1</v>
       </c>
       <c r="H38" s="12">
-        <f t="shared" ref="H38" si="8">F38*G38</f>
+        <f t="shared" ref="H38:H40" si="8">F38*G38</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A39" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="24"/>
+    <row r="39" spans="1:8" ht="42.75">
+      <c r="A39" s="7">
+        <v>12</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G39" s="11">
+        <v>4</v>
+      </c>
+      <c r="H39" s="12">
+        <f t="shared" si="8"/>
+        <v>0.44</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="42.75">
       <c r="A40" s="7">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1</v>
+      </c>
+      <c r="H40" s="12">
+        <f t="shared" si="8"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A41" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="26"/>
+    </row>
+    <row r="42" spans="1:8" ht="42.75">
+      <c r="A42" s="7">
+        <v>1</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" s="10">
+      <c r="E42" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="10">
         <v>0.88</v>
       </c>
-      <c r="G40" s="11">
-        <v>1</v>
-      </c>
-      <c r="H40" s="12">
-        <f t="shared" ref="H40:H80" si="9">F40*G40</f>
+      <c r="G42" s="11">
+        <v>1</v>
+      </c>
+      <c r="H42" s="12">
+        <f t="shared" ref="H42:H82" si="9">F42*G42</f>
         <v>0.88</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="42.75">
-      <c r="A41" s="7">
+    <row r="43" spans="1:8" ht="42.75">
+      <c r="A43" s="7">
         <v>2</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B43" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="10">
+      <c r="E43" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="10">
         <v>0.88</v>
       </c>
-      <c r="G41" s="11">
-        <v>1</v>
-      </c>
-      <c r="H41" s="12">
+      <c r="G43" s="11">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12">
         <f t="shared" si="9"/>
         <v>0.88</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="42.75">
-      <c r="A42" s="7">
+    <row r="44" spans="1:8" ht="42.75">
+      <c r="A44" s="7">
         <v>3</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="13" t="s">
+      <c r="B44" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="10">
+      <c r="D44" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="10">
         <v>0.22</v>
       </c>
-      <c r="G42" s="11">
-        <v>1</v>
-      </c>
-      <c r="H42" s="12">
+      <c r="G44" s="11">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12">
         <f t="shared" si="9"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="7">
+    <row r="45" spans="1:8" ht="42.75">
+      <c r="A45" s="7">
         <v>4</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="13" t="s">
+      <c r="B45" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F43" s="10">
+      <c r="D45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="10">
         <v>0.22</v>
       </c>
-      <c r="G43" s="11">
-        <v>1</v>
-      </c>
-      <c r="H43" s="12">
+      <c r="G45" s="11">
+        <v>1</v>
+      </c>
+      <c r="H45" s="12">
         <f t="shared" si="9"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="42.75">
-      <c r="A44" s="7">
+    <row r="46" spans="1:8" ht="42.75">
+      <c r="A46" s="7">
         <v>5</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="10">
+      <c r="B46" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="10">
         <v>0.44</v>
       </c>
-      <c r="G44" s="11">
-        <v>1</v>
-      </c>
-      <c r="H44" s="12">
+      <c r="G46" s="11">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12">
         <f t="shared" si="9"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="42.75">
-      <c r="A45" s="7">
+    <row r="47" spans="1:8" ht="42.75">
+      <c r="A47" s="7">
         <v>6</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="13" t="s">
+      <c r="B47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="10">
+      <c r="F47" s="10">
         <v>0.44</v>
       </c>
-      <c r="G45" s="11">
-        <v>1</v>
-      </c>
-      <c r="H45" s="12">
+      <c r="G47" s="11">
+        <v>1</v>
+      </c>
+      <c r="H47" s="12">
         <f t="shared" si="9"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="42.75">
-      <c r="A46" s="7">
+    <row r="48" spans="1:8" ht="42.75">
+      <c r="A48" s="7">
         <v>7</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="B48" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="E48" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="10">
+      <c r="F48" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G46" s="11">
-        <v>1</v>
-      </c>
-      <c r="H46" s="12">
+      <c r="G48" s="11">
+        <v>1</v>
+      </c>
+      <c r="H48" s="12">
         <f t="shared" si="9"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42.75">
-      <c r="A47" s="7">
+    <row r="49" spans="1:8" ht="42.75">
+      <c r="A49" s="7">
         <v>8</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="B49" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="E49" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="10">
+      <c r="F49" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G47" s="11">
-        <v>1</v>
-      </c>
-      <c r="H47" s="12">
+      <c r="G49" s="11">
+        <v>1</v>
+      </c>
+      <c r="H49" s="12">
         <f t="shared" si="9"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="42.75">
-      <c r="A48" s="7">
+    <row r="50" spans="1:8" ht="42.75">
+      <c r="A50" s="7">
         <v>9</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="B50" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="F50" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1</v>
+      </c>
+      <c r="H50" s="12">
+        <f t="shared" ref="H50:H59" si="10">F50*G50</f>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="42.75">
+      <c r="A51" s="7">
+        <v>10</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="10">
+      <c r="C51" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="10">
         <v>0.54</v>
       </c>
-      <c r="G48" s="11">
-        <v>1</v>
-      </c>
-      <c r="H48" s="12">
-        <f t="shared" ref="H48:H57" si="10">F48*G48</f>
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="42.75">
-      <c r="A49" s="7">
-        <v>10</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F49" s="10">
-        <v>0.54</v>
-      </c>
-      <c r="G49" s="11">
-        <v>1</v>
-      </c>
-      <c r="H49" s="12">
+      <c r="G51" s="11">
+        <v>1</v>
+      </c>
+      <c r="H51" s="12">
         <f t="shared" si="10"/>
         <v>0.54</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="42.75">
-      <c r="A50" s="7">
+    <row r="52" spans="1:8" ht="42.75">
+      <c r="A52" s="7">
         <v>11</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C50" s="7" t="s">
+      <c r="B52" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" s="13"/>
+      <c r="E52" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F50" s="10">
+      <c r="F52" s="10">
         <v>0.66</v>
       </c>
-      <c r="G50" s="11">
-        <v>1</v>
-      </c>
-      <c r="H50" s="12">
+      <c r="G52" s="11">
+        <v>1</v>
+      </c>
+      <c r="H52" s="12">
         <f t="shared" si="10"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="42.75">
-      <c r="A51" s="7">
+    <row r="53" spans="1:8" ht="42.75">
+      <c r="A53" s="7">
         <v>12</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="B53" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F51" s="10">
+      <c r="F53" s="10">
         <v>0.66</v>
       </c>
-      <c r="G51" s="11">
-        <v>1</v>
-      </c>
-      <c r="H51" s="12">
+      <c r="G53" s="11">
+        <v>1</v>
+      </c>
+      <c r="H53" s="12">
         <f t="shared" si="10"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="42.75">
-      <c r="A52" s="7">
+    <row r="54" spans="1:8" ht="42.75">
+      <c r="A54" s="7">
         <v>13</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C52" s="7" t="s">
+      <c r="B54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="13"/>
+      <c r="E54" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D52" s="13"/>
-      <c r="E52" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F52" s="10">
+      <c r="F54" s="10">
         <v>0.44</v>
       </c>
-      <c r="G52" s="11">
-        <v>1</v>
-      </c>
-      <c r="H52" s="12">
+      <c r="G54" s="11">
+        <v>1</v>
+      </c>
+      <c r="H54" s="12">
         <f t="shared" si="10"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="42.75">
-      <c r="A53" s="7">
+    <row r="55" spans="1:8" ht="42.75">
+      <c r="A55" s="7">
         <v>14</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="7" t="s">
+      <c r="B55" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D55" s="13"/>
+      <c r="E55" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F53" s="10">
+      <c r="F55" s="10">
         <v>0.44</v>
       </c>
-      <c r="G53" s="11">
-        <v>1</v>
-      </c>
-      <c r="H53" s="12">
+      <c r="G55" s="11">
+        <v>1</v>
+      </c>
+      <c r="H55" s="12">
         <f t="shared" si="10"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42.75">
-      <c r="A54" s="7">
+    <row r="56" spans="1:8" ht="42.75">
+      <c r="A56" s="7">
         <v>15</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C54" s="7" t="s">
+      <c r="B56" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="13"/>
-      <c r="E54" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F54" s="10">
+      <c r="F56" s="10">
         <v>1.21</v>
       </c>
-      <c r="G54" s="11">
-        <v>1</v>
-      </c>
-      <c r="H54" s="12">
+      <c r="G56" s="11">
+        <v>1</v>
+      </c>
+      <c r="H56" s="12">
         <f t="shared" si="10"/>
         <v>1.21</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="42.75">
-      <c r="A55" s="7">
+    <row r="57" spans="1:8" ht="42.75">
+      <c r="A57" s="7">
         <v>16</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B57" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="D57" s="13"/>
+      <c r="E57" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F55" s="10">
+      <c r="F57" s="10">
         <v>1.21</v>
       </c>
-      <c r="G55" s="11">
-        <v>1</v>
-      </c>
-      <c r="H55" s="12">
+      <c r="G57" s="11">
+        <v>1</v>
+      </c>
+      <c r="H57" s="12">
         <f t="shared" si="10"/>
         <v>1.21</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="42.75">
-      <c r="A56" s="7">
+    <row r="58" spans="1:8" ht="42.75">
+      <c r="A58" s="7">
         <v>17</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C56" s="7" t="s">
+      <c r="B58" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="13"/>
+      <c r="E58" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F56" s="10">
+      <c r="F58" s="10">
         <v>0.44</v>
       </c>
-      <c r="G56" s="11">
-        <v>1</v>
-      </c>
-      <c r="H56" s="12">
+      <c r="G58" s="11">
+        <v>1</v>
+      </c>
+      <c r="H58" s="12">
         <f t="shared" si="10"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="42.75">
-      <c r="A57" s="7">
+    <row r="59" spans="1:8" ht="42.75">
+      <c r="A59" s="7">
         <v>18</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="7" t="s">
+      <c r="B59" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" s="13"/>
+      <c r="E59" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D57" s="13"/>
-      <c r="E57" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F57" s="10">
+      <c r="F59" s="10">
         <v>0.44</v>
       </c>
-      <c r="G57" s="11">
-        <v>1</v>
-      </c>
-      <c r="H57" s="12">
+      <c r="G59" s="11">
+        <v>1</v>
+      </c>
+      <c r="H59" s="12">
         <f t="shared" si="10"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="42.75">
-      <c r="A58" s="7">
+    <row r="60" spans="1:8" ht="42.75">
+      <c r="A60" s="7">
         <v>19</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B60" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="13"/>
+      <c r="E60" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="10">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G60" s="11">
+        <v>1</v>
+      </c>
+      <c r="H60" s="12">
+        <f t="shared" ref="H60:H61" si="11">F60*G60</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="42.75">
+      <c r="A61" s="7">
+        <v>20</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C61" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" s="13"/>
+      <c r="E61" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="F58" s="10">
+      <c r="F61" s="10">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G58" s="11">
-        <v>1</v>
-      </c>
-      <c r="H58" s="12">
-        <f t="shared" ref="H58:H59" si="11">F58*G58</f>
-        <v>0.16500000000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="42.75">
-      <c r="A59" s="7">
-        <v>20</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="F59" s="10">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G59" s="11">
-        <v>1</v>
-      </c>
-      <c r="H59" s="12">
+      <c r="G61" s="11">
+        <v>1</v>
+      </c>
+      <c r="H61" s="12">
         <f t="shared" si="11"/>
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="57">
-      <c r="A60" s="7">
-        <v>21</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F60" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G60" s="11">
-        <v>1</v>
-      </c>
-      <c r="H60" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="57">
-      <c r="A61" s="7">
-        <v>22</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F61" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G61" s="11">
-        <v>1</v>
-      </c>
-      <c r="H61" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
     <row r="62" spans="1:8" ht="57">
       <c r="A62" s="7">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C62" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="E62" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F62" s="10">
         <v>0.11</v>
@@ -2829,19 +2916,19 @@
     </row>
     <row r="63" spans="1:8" ht="57">
       <c r="A63" s="7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F63" s="10">
         <v>0.11</v>
@@ -2856,19 +2943,19 @@
     </row>
     <row r="64" spans="1:8" ht="57">
       <c r="A64" s="7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F64" s="10">
         <v>0.11</v>
@@ -2881,21 +2968,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="71.25">
+    <row r="65" spans="1:8" ht="57">
       <c r="A65" s="7">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F65" s="10">
         <v>0.11</v>
@@ -2910,19 +2997,19 @@
     </row>
     <row r="66" spans="1:8" ht="57">
       <c r="A66" s="7">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F66" s="10">
         <v>0.11</v>
@@ -2935,21 +3022,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="42.75">
+    <row r="67" spans="1:8" ht="71.25">
       <c r="A67" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F67" s="10">
         <v>0.11</v>
@@ -2964,19 +3051,19 @@
     </row>
     <row r="68" spans="1:8" ht="57">
       <c r="A68" s="7">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F68" s="10">
         <v>0.11</v>
@@ -2989,21 +3076,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="57">
+    <row r="69" spans="1:8" ht="42.75">
       <c r="A69" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>135</v>
+        <v>116</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F69" s="10">
         <v>0.11</v>
@@ -3018,19 +3105,19 @@
     </row>
     <row r="70" spans="1:8" ht="57">
       <c r="A70" s="7">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F70" s="10">
         <v>0.11</v>
@@ -3045,19 +3132,19 @@
     </row>
     <row r="71" spans="1:8" ht="57">
       <c r="A71" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F71" s="10">
         <v>0.11</v>
@@ -3072,19 +3159,19 @@
     </row>
     <row r="72" spans="1:8" ht="57">
       <c r="A72" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F72" s="10">
         <v>0.11</v>
@@ -3099,19 +3186,19 @@
     </row>
     <row r="73" spans="1:8" ht="57">
       <c r="A73" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>142</v>
+        <v>116</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F73" s="10">
         <v>0.11</v>
@@ -3126,19 +3213,19 @@
     </row>
     <row r="74" spans="1:8" ht="57">
       <c r="A74" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>144</v>
+        <v>116</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F74" s="10">
         <v>0.11</v>
@@ -3151,21 +3238,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="71.25">
+    <row r="75" spans="1:8" ht="57">
       <c r="A75" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F75" s="10">
         <v>0.11</v>
@@ -3180,19 +3267,19 @@
     </row>
     <row r="76" spans="1:8" ht="57">
       <c r="A76" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F76" s="10">
         <v>0.11</v>
@@ -3205,21 +3292,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="57">
+    <row r="77" spans="1:8" ht="71.25">
       <c r="A77" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F77" s="10">
         <v>0.11</v>
@@ -3232,21 +3319,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="71.25">
+    <row r="78" spans="1:8" ht="57">
       <c r="A78" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>150</v>
+        <v>116</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F78" s="10">
         <v>0.11</v>
@@ -3261,19 +3348,19 @@
     </row>
     <row r="79" spans="1:8" ht="57">
       <c r="A79" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F79" s="10">
         <v>0.11</v>
@@ -3286,21 +3373,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="57">
+    <row r="80" spans="1:8" ht="71.25">
       <c r="A80" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F80" s="10">
         <v>0.11</v>
@@ -3313,985 +3400,1247 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="42.75">
+    <row r="81" spans="1:8" ht="57">
       <c r="A81" s="7">
+        <v>40</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F81" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G81" s="11">
+        <v>1</v>
+      </c>
+      <c r="H81" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="57">
+      <c r="A82" s="7">
+        <v>41</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F82" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G82" s="11">
+        <v>1</v>
+      </c>
+      <c r="H82" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="42.75">
+      <c r="A83" s="7">
         <v>42</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B83" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="13"/>
+      <c r="E83" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F83" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="G83" s="11">
+        <v>1</v>
+      </c>
+      <c r="H83" s="12">
+        <f t="shared" ref="H83:H103" si="12">F83*G83</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="42.75">
+      <c r="A84" s="7">
+        <v>43</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C81" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D81" s="13"/>
-      <c r="E81" s="9" t="s">
+      <c r="C84" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="13"/>
+      <c r="E84" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F81" s="10">
-        <v>0.88</v>
-      </c>
-      <c r="G81" s="11">
-        <v>1</v>
-      </c>
-      <c r="H81" s="12">
-        <f t="shared" ref="H81:H89" si="12">F81*G81</f>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" ht="42.75">
-      <c r="A82" s="7">
-        <v>43</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F82" s="10">
+      <c r="F84" s="10">
         <v>0.22</v>
       </c>
-      <c r="G82" s="11">
-        <v>1</v>
-      </c>
-      <c r="H82" s="12">
+      <c r="G84" s="11">
+        <v>1</v>
+      </c>
+      <c r="H84" s="12">
         <f t="shared" si="12"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="42.75">
-      <c r="A83" s="7">
+    <row r="85" spans="1:8" ht="42.75">
+      <c r="A85" s="7">
         <v>44</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D83" s="13"/>
-      <c r="E83" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F83" s="10">
+      <c r="B85" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D85" s="13"/>
+      <c r="E85" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F85" s="10">
         <v>0.44</v>
       </c>
-      <c r="G83" s="11">
-        <v>1</v>
-      </c>
-      <c r="H83" s="12">
+      <c r="G85" s="11">
+        <v>1</v>
+      </c>
+      <c r="H85" s="12">
         <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="42.75">
-      <c r="A84" s="7">
+    <row r="86" spans="1:8" ht="42.75">
+      <c r="A86" s="7">
         <v>45</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D84" s="13"/>
-      <c r="E84" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F84" s="10">
+      <c r="B86" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D86" s="13"/>
+      <c r="E86" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F86" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G84" s="11">
-        <v>1</v>
-      </c>
-      <c r="H84" s="12">
+      <c r="G86" s="11">
+        <v>1</v>
+      </c>
+      <c r="H86" s="12">
         <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="42.75">
-      <c r="A85" s="7">
+    <row r="87" spans="1:8" ht="42.75">
+      <c r="A87" s="7">
         <v>46</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C85" s="7" t="s">
+      <c r="B87" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="13"/>
+      <c r="E87" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D85" s="13"/>
-      <c r="E85" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F85" s="10">
+      <c r="F87" s="10">
         <v>0.54</v>
       </c>
-      <c r="G85" s="11">
-        <v>1</v>
-      </c>
-      <c r="H85" s="12">
+      <c r="G87" s="11">
+        <v>1</v>
+      </c>
+      <c r="H87" s="12">
         <f t="shared" si="12"/>
         <v>0.54</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="42.75">
-      <c r="A86" s="7">
+    <row r="88" spans="1:8" ht="42.75">
+      <c r="A88" s="7">
         <v>47</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C86" s="7" t="s">
+      <c r="B88" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" s="13"/>
+      <c r="E88" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D86" s="13"/>
-      <c r="E86" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F86" s="10">
+      <c r="F88" s="10">
         <v>0.66</v>
       </c>
-      <c r="G86" s="11">
-        <v>1</v>
-      </c>
-      <c r="H86" s="12">
+      <c r="G88" s="11">
+        <v>1</v>
+      </c>
+      <c r="H88" s="12">
         <f t="shared" si="12"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="42.75">
-      <c r="A87" s="7">
+    <row r="89" spans="1:8" ht="42.75">
+      <c r="A89" s="7">
         <v>48</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="7" t="s">
+      <c r="B89" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" s="13"/>
+      <c r="E89" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D87" s="13"/>
-      <c r="E87" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F87" s="10">
+      <c r="F89" s="10">
         <v>0.44</v>
       </c>
-      <c r="G87" s="11">
-        <v>1</v>
-      </c>
-      <c r="H87" s="12">
+      <c r="G89" s="11">
+        <v>1</v>
+      </c>
+      <c r="H89" s="12">
         <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="42.75">
-      <c r="A88" s="7">
+    <row r="90" spans="1:8" ht="42.75">
+      <c r="A90" s="7">
         <v>49</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="7" t="s">
+      <c r="B90" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D90" s="13"/>
+      <c r="E90" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D88" s="13"/>
-      <c r="E88" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F88" s="10">
+      <c r="F90" s="10">
         <v>1.21</v>
       </c>
-      <c r="G88" s="11">
-        <v>1</v>
-      </c>
-      <c r="H88" s="12">
+      <c r="G90" s="11">
+        <v>1</v>
+      </c>
+      <c r="H90" s="12">
         <f t="shared" si="12"/>
         <v>1.21</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="42.75">
-      <c r="A89" s="7">
+    <row r="91" spans="1:8" ht="42.75">
+      <c r="A91" s="7">
         <v>50</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C89" s="7" t="s">
+      <c r="B91" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91" s="13"/>
+      <c r="E91" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D89" s="13"/>
-      <c r="E89" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="F89" s="10">
+      <c r="F91" s="10">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G89" s="11">
-        <v>1</v>
-      </c>
-      <c r="H89" s="12">
+      <c r="G91" s="11">
+        <v>1</v>
+      </c>
+      <c r="H91" s="12">
         <f t="shared" si="12"/>
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:22" ht="14.25" customHeight="1">
-      <c r="A90" s="27" t="s">
+    <row r="92" spans="1:8" ht="57">
+      <c r="A92" s="7">
+        <v>51</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F92" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G92" s="11">
+        <v>1</v>
+      </c>
+      <c r="H92" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="57">
+      <c r="A93" s="7">
+        <v>52</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F93" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G93" s="11">
+        <v>1</v>
+      </c>
+      <c r="H93" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="57">
+      <c r="A94" s="7">
+        <v>53</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G94" s="11">
+        <v>1</v>
+      </c>
+      <c r="H94" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="57">
+      <c r="A95" s="7">
+        <v>54</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F95" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G95" s="11">
+        <v>1</v>
+      </c>
+      <c r="H95" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="71.25">
+      <c r="A96" s="7">
+        <v>55</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D96" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F96" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G96" s="11">
+        <v>1</v>
+      </c>
+      <c r="H96" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" ht="57">
+      <c r="A97" s="7">
+        <v>56</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D97" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F97" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G97" s="11">
+        <v>1</v>
+      </c>
+      <c r="H97" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22" ht="57">
+      <c r="A98" s="7">
+        <v>57</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D98" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F98" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G98" s="11">
+        <v>1</v>
+      </c>
+      <c r="H98" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" ht="57">
+      <c r="A99" s="7">
+        <v>58</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F99" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1</v>
+      </c>
+      <c r="H99" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" ht="57">
+      <c r="A100" s="7">
+        <v>59</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F100" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G100" s="11">
+        <v>1</v>
+      </c>
+      <c r="H100" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" ht="71.25">
+      <c r="A101" s="7">
+        <v>60</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F101" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G101" s="11">
+        <v>1</v>
+      </c>
+      <c r="H101" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" ht="57">
+      <c r="A102" s="7">
+        <v>61</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F102" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G102" s="11">
+        <v>1</v>
+      </c>
+      <c r="H102" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" ht="57">
+      <c r="A103" s="7">
+        <v>62</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F103" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G103" s="11">
+        <v>1</v>
+      </c>
+      <c r="H103" s="12">
+        <f t="shared" si="12"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" ht="14.25" customHeight="1">
+      <c r="A104" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="15"/>
+      <c r="O104" s="15"/>
+      <c r="P104" s="15"/>
+      <c r="Q104" s="15"/>
+      <c r="R104" s="15"/>
+      <c r="S104" s="15"/>
+      <c r="T104" s="15"/>
+      <c r="U104" s="15"/>
+      <c r="V104" s="15"/>
+    </row>
+    <row r="105" spans="1:22" ht="28.5">
+      <c r="A105" s="16">
+        <v>1</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="E105" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F105" s="16">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G105" s="16">
+        <v>18</v>
+      </c>
+      <c r="H105" s="16">
+        <f>F105*G105</f>
+        <v>2.97</v>
+      </c>
+      <c r="I105" s="15"/>
+      <c r="J105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="15"/>
+      <c r="N105" s="15"/>
+      <c r="O105" s="15"/>
+      <c r="P105" s="15"/>
+      <c r="Q105" s="15"/>
+      <c r="R105" s="15"/>
+      <c r="S105" s="15"/>
+      <c r="T105" s="15"/>
+      <c r="U105" s="15"/>
+      <c r="V105" s="15"/>
+    </row>
+    <row r="106" spans="1:22" ht="42.75">
+      <c r="A106" s="16">
+        <v>2</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C106" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="29"/>
-      <c r="I90" s="15"/>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="15"/>
-      <c r="M90" s="15"/>
-      <c r="N90" s="15"/>
-      <c r="O90" s="15"/>
-      <c r="P90" s="15"/>
-      <c r="Q90" s="15"/>
-      <c r="R90" s="15"/>
-      <c r="S90" s="15"/>
-      <c r="T90" s="15"/>
-      <c r="U90" s="15"/>
-      <c r="V90" s="15"/>
-    </row>
-    <row r="91" spans="1:22" ht="28.5">
-      <c r="A91" s="16">
-        <v>1</v>
-      </c>
-      <c r="B91" s="17" t="s">
+      <c r="D106" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F106" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="G106" s="16">
+        <v>52</v>
+      </c>
+      <c r="H106" s="16">
+        <f>F106*G106</f>
+        <v>4.16</v>
+      </c>
+      <c r="I106" s="15"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="15"/>
+      <c r="M106" s="15"/>
+      <c r="N106" s="15"/>
+      <c r="O106" s="15"/>
+      <c r="P106" s="15"/>
+      <c r="Q106" s="15"/>
+      <c r="R106" s="15"/>
+      <c r="S106" s="15"/>
+      <c r="T106" s="15"/>
+      <c r="U106" s="15"/>
+      <c r="V106" s="15"/>
+    </row>
+    <row r="107" spans="1:22" ht="42.75">
+      <c r="A107" s="16">
+        <v>3</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F107" s="16">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G107" s="16">
+        <v>18</v>
+      </c>
+      <c r="H107" s="16">
+        <f>F107*G107</f>
+        <v>2.97</v>
+      </c>
+      <c r="I107" s="15"/>
+      <c r="J107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="15"/>
+      <c r="M107" s="15"/>
+      <c r="N107" s="15"/>
+      <c r="O107" s="15"/>
+      <c r="P107" s="15"/>
+      <c r="Q107" s="15"/>
+      <c r="R107" s="15"/>
+      <c r="S107" s="15"/>
+      <c r="T107" s="15"/>
+      <c r="U107" s="15"/>
+      <c r="V107" s="15"/>
+    </row>
+    <row r="108" spans="1:22" ht="42.75">
+      <c r="A108" s="16">
+        <v>4</v>
+      </c>
+      <c r="B108" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C108" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F108" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="G108" s="16">
+        <v>52</v>
+      </c>
+      <c r="H108" s="16">
+        <f>F108*G108</f>
+        <v>4.16</v>
+      </c>
+      <c r="I108" s="15"/>
+      <c r="J108" s="15"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="15"/>
+      <c r="M108" s="15"/>
+      <c r="N108" s="15"/>
+      <c r="O108" s="15"/>
+      <c r="P108" s="15"/>
+      <c r="Q108" s="15"/>
+      <c r="R108" s="15"/>
+      <c r="S108" s="15"/>
+      <c r="T108" s="15"/>
+      <c r="U108" s="15"/>
+      <c r="V108" s="15"/>
+    </row>
+    <row r="109" spans="1:22" ht="15" customHeight="1">
+      <c r="A109" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="25"/>
+      <c r="H109" s="26"/>
+    </row>
+    <row r="110" spans="1:22" ht="42.75">
+      <c r="A110" s="7">
+        <v>1</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F110" s="10">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G110" s="11">
+        <v>1</v>
+      </c>
+      <c r="H110" s="16">
+        <f>F110*G110</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22" ht="57">
+      <c r="A111" s="7">
+        <v>2</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F111" s="10">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G111" s="11">
+        <v>1</v>
+      </c>
+      <c r="H111" s="12">
+        <f>F111*G111</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:22">
+      <c r="A112" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="25"/>
+      <c r="H112" s="26"/>
+    </row>
+    <row r="113" spans="1:8" ht="57">
+      <c r="A113" s="7">
+        <v>1</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D91" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E91" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F91" s="16">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G91" s="16">
-        <v>18</v>
-      </c>
-      <c r="H91" s="16">
-        <f>F91*G91</f>
-        <v>2.97</v>
-      </c>
-      <c r="I91" s="15"/>
-      <c r="J91" s="15"/>
-      <c r="K91" s="15"/>
-      <c r="L91" s="15"/>
-      <c r="M91" s="15"/>
-      <c r="N91" s="15"/>
-      <c r="O91" s="15"/>
-      <c r="P91" s="15"/>
-      <c r="Q91" s="15"/>
-      <c r="R91" s="15"/>
-      <c r="S91" s="15"/>
-      <c r="T91" s="15"/>
-      <c r="U91" s="15"/>
-      <c r="V91" s="15"/>
-    </row>
-    <row r="92" spans="1:22" ht="42.75">
-      <c r="A92" s="16">
+      <c r="D113" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F113" s="10">
+        <v>1</v>
+      </c>
+      <c r="G113" s="11">
+        <v>1</v>
+      </c>
+      <c r="H113" s="16">
+        <f t="shared" ref="H113:H125" si="13">F113*G113</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="42.75">
+      <c r="A114" s="7">
         <v>2</v>
       </c>
-      <c r="B92" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E92" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="G92" s="16">
-        <v>52</v>
-      </c>
-      <c r="H92" s="16">
-        <f>F92*G92</f>
-        <v>4.16</v>
-      </c>
-      <c r="I92" s="15"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
-      <c r="L92" s="15"/>
-      <c r="M92" s="15"/>
-      <c r="N92" s="15"/>
-      <c r="O92" s="15"/>
-      <c r="P92" s="15"/>
-      <c r="Q92" s="15"/>
-      <c r="R92" s="15"/>
-      <c r="S92" s="15"/>
-      <c r="T92" s="15"/>
-      <c r="U92" s="15"/>
-      <c r="V92" s="15"/>
-    </row>
-    <row r="93" spans="1:22" ht="42.75">
-      <c r="A93" s="16">
+      <c r="B114" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D114" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F114" s="10">
+        <v>1</v>
+      </c>
+      <c r="G114" s="11">
+        <v>1</v>
+      </c>
+      <c r="H114" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="42.75">
+      <c r="A115" s="7">
         <v>3</v>
       </c>
-      <c r="B93" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C93" s="19" t="s">
+      <c r="B115" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C115" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D93" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="E93" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F93" s="16">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="G93" s="16">
-        <v>18</v>
-      </c>
-      <c r="H93" s="16">
-        <f>F93*G93</f>
-        <v>2.97</v>
-      </c>
-      <c r="I93" s="15"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-      <c r="L93" s="15"/>
-      <c r="M93" s="15"/>
-      <c r="N93" s="15"/>
-      <c r="O93" s="15"/>
-      <c r="P93" s="15"/>
-      <c r="Q93" s="15"/>
-      <c r="R93" s="15"/>
-      <c r="S93" s="15"/>
-      <c r="T93" s="15"/>
-      <c r="U93" s="15"/>
-      <c r="V93" s="15"/>
-    </row>
-    <row r="94" spans="1:22" ht="42.75">
-      <c r="A94" s="16">
+      <c r="D115" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F115" s="10">
+        <v>1</v>
+      </c>
+      <c r="G115" s="11">
+        <v>1</v>
+      </c>
+      <c r="H115" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="42.75">
+      <c r="A116" s="7">
         <v>4</v>
       </c>
-      <c r="B94" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="E94" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F94" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="G94" s="16">
-        <v>52</v>
-      </c>
-      <c r="H94" s="16">
-        <f>F94*G94</f>
-        <v>4.16</v>
-      </c>
-      <c r="I94" s="15"/>
-      <c r="J94" s="15"/>
-      <c r="K94" s="15"/>
-      <c r="L94" s="15"/>
-      <c r="M94" s="15"/>
-      <c r="N94" s="15"/>
-      <c r="O94" s="15"/>
-      <c r="P94" s="15"/>
-      <c r="Q94" s="15"/>
-      <c r="R94" s="15"/>
-      <c r="S94" s="15"/>
-      <c r="T94" s="15"/>
-      <c r="U94" s="15"/>
-      <c r="V94" s="15"/>
-    </row>
-    <row r="95" spans="1:22" ht="15" customHeight="1">
-      <c r="A95" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B95" s="23"/>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="23"/>
-      <c r="H95" s="24"/>
-    </row>
-    <row r="96" spans="1:22">
-      <c r="A96" s="7">
-        <v>1</v>
-      </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="12"/>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
-      <c r="H97" s="24"/>
-    </row>
-    <row r="98" spans="1:8" ht="57">
-      <c r="A98" s="7">
-        <v>1</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D98" s="13" t="s">
+      <c r="B116" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E98" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F98" s="10">
-        <v>1</v>
-      </c>
-      <c r="G98" s="11">
-        <v>1</v>
-      </c>
-      <c r="H98" s="16">
-        <f t="shared" ref="H98:H110" si="13">F98*G98</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="42.75">
-      <c r="A99" s="7">
-        <v>2</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D99" s="13" t="s">
+      <c r="D116" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E116" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E99" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F99" s="10">
-        <v>1</v>
-      </c>
-      <c r="G99" s="11">
-        <v>1</v>
-      </c>
-      <c r="H99" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="42.75">
-      <c r="A100" s="7">
-        <v>3</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D100" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F100" s="10">
-        <v>1</v>
-      </c>
-      <c r="G100" s="11">
-        <v>1</v>
-      </c>
-      <c r="H100" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="42.75">
-      <c r="A101" s="7">
-        <v>4</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F101" s="10">
+      <c r="F116" s="10">
         <v>0.5</v>
       </c>
-      <c r="G101" s="11">
-        <v>1</v>
-      </c>
-      <c r="H101" s="16">
-        <f t="shared" ref="H101" si="14">F101*G101</f>
+      <c r="G116" s="11">
+        <v>1</v>
+      </c>
+      <c r="H116" s="16">
+        <f t="shared" ref="H116" si="14">F116*G116</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="57">
-      <c r="A102" s="7">
+    <row r="117" spans="1:8" ht="57">
+      <c r="A117" s="7">
         <v>5</v>
       </c>
-      <c r="B102" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F102" s="10">
+      <c r="B117" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D117" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F117" s="10">
         <v>0.5</v>
       </c>
-      <c r="G102" s="11">
-        <v>1</v>
-      </c>
-      <c r="H102" s="16">
+      <c r="G117" s="11">
+        <v>1</v>
+      </c>
+      <c r="H117" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="42.75">
-      <c r="A103" s="7">
+    <row r="118" spans="1:8" ht="42.75">
+      <c r="A118" s="7">
         <v>6</v>
       </c>
-      <c r="B103" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D103" s="13" t="s">
+      <c r="B118" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D118" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F118" s="10">
+        <v>1</v>
+      </c>
+      <c r="G118" s="11">
+        <v>1</v>
+      </c>
+      <c r="H118" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="57">
+      <c r="A119" s="7">
+        <v>7</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="E103" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F103" s="10">
-        <v>1</v>
-      </c>
-      <c r="G103" s="11">
-        <v>1</v>
-      </c>
-      <c r="H103" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="57">
-      <c r="A104" s="7">
-        <v>7</v>
-      </c>
-      <c r="B104" s="8" t="s">
+      <c r="C119" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D119" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="C104" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F104" s="10">
+      <c r="E119" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F119" s="10">
         <v>0.5</v>
       </c>
-      <c r="G104" s="11">
-        <v>1</v>
-      </c>
-      <c r="H104" s="16">
+      <c r="G119" s="11">
+        <v>1</v>
+      </c>
+      <c r="H119" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="42.75">
-      <c r="A105" s="7">
+    <row r="120" spans="1:8" ht="42.75">
+      <c r="A120" s="7">
         <v>8</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B120" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D120" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="C105" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D105" s="13" t="s">
+      <c r="E120" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F120" s="10">
+        <v>1</v>
+      </c>
+      <c r="G120" s="11">
+        <v>1</v>
+      </c>
+      <c r="H120" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="42.75">
+      <c r="A121" s="7">
+        <v>9</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F121" s="10">
+        <v>1</v>
+      </c>
+      <c r="G121" s="11">
+        <v>1</v>
+      </c>
+      <c r="H121" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="57">
+      <c r="A122" s="7">
+        <v>10</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F122" s="10">
+        <v>1</v>
+      </c>
+      <c r="G122" s="11">
+        <v>1</v>
+      </c>
+      <c r="H122" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="57">
+      <c r="A123" s="7">
+        <v>11</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E105" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F105" s="10">
-        <v>1</v>
-      </c>
-      <c r="G105" s="11">
-        <v>1</v>
-      </c>
-      <c r="H105" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="42.75">
-      <c r="A106" s="7">
-        <v>9</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D106" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F106" s="10">
-        <v>1</v>
-      </c>
-      <c r="G106" s="11">
-        <v>1</v>
-      </c>
-      <c r="H106" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="57">
-      <c r="A107" s="7">
-        <v>10</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F107" s="10">
-        <v>1</v>
-      </c>
-      <c r="G107" s="11">
-        <v>1</v>
-      </c>
-      <c r="H107" s="16">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="57">
-      <c r="A108" s="7">
-        <v>11</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D108" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F108" s="10">
+      <c r="C123" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E123" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F123" s="10">
         <v>0.5</v>
       </c>
-      <c r="G108" s="11">
-        <v>1</v>
-      </c>
-      <c r="H108" s="16">
+      <c r="G123" s="11">
+        <v>1</v>
+      </c>
+      <c r="H123" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="42.75">
-      <c r="A109" s="7">
+    <row r="124" spans="1:8" ht="42.75">
+      <c r="A124" s="7">
         <v>12</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D109" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F109" s="10">
+      <c r="B124" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D124" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E124" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F124" s="10">
         <v>0.5</v>
       </c>
-      <c r="G109" s="11">
-        <v>1</v>
-      </c>
-      <c r="H109" s="16">
+      <c r="G124" s="11">
+        <v>1</v>
+      </c>
+      <c r="H124" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="57">
-      <c r="A110" s="7">
+    <row r="125" spans="1:8" ht="57">
+      <c r="A125" s="7">
         <v>13</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B125" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D125" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C110" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D110" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F110" s="10">
+      <c r="E125" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F125" s="10">
         <v>0.5</v>
       </c>
-      <c r="G110" s="11">
-        <v>1</v>
-      </c>
-      <c r="H110" s="16">
+      <c r="G125" s="11">
+        <v>1</v>
+      </c>
+      <c r="H125" s="16">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
-      <c r="A111" s="26" t="s">
+    <row r="126" spans="1:8">
+      <c r="A126" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="26"/>
-      <c r="H111" s="6">
-        <f>SUM(H23:H110)</f>
-        <v>73.544999999999945</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="1" t="s">
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="6">
+        <f>SUM(H23:H125)</f>
+        <v>75.744999999999962</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8">
-      <c r="A113" s="1"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-    </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="1"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G114" s="20"/>
-      <c r="H114" s="20"/>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="1"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="1"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8">
-      <c r="A117" s="1"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="1:8">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="1"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G119" s="20"/>
-      <c r="H119" s="20"/>
-    </row>
-    <row r="120" spans="1:8">
-      <c r="A120" s="1"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G120" s="20"/>
-      <c r="H120" s="20"/>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="1"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="1"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-    </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="1"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8">
-      <c r="A124" s="1"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="1"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8">
-      <c r="A126" s="1"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-    </row>
-    <row r="127" spans="1:8">
-      <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -4306,9 +4655,11 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
-      <c r="G128" s="1"/>
-      <c r="H128" s="1"/>
+      <c r="F128" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G128" s="22"/>
+      <c r="H128" s="22"/>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="1"/>
@@ -4316,9 +4667,11 @@
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="1"/>
+      <c r="F129" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G129" s="22"/>
+      <c r="H129" s="22"/>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" s="1"/>
@@ -4366,9 +4719,11 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
-      <c r="H134" s="1"/>
+      <c r="F134" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G134" s="22"/>
+      <c r="H134" s="22"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="1"/>
@@ -4376,9 +4731,11 @@
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
-      <c r="G135" s="1"/>
-      <c r="H135" s="1"/>
+      <c r="F135" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G135" s="22"/>
+      <c r="H135" s="22"/>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="1"/>
@@ -4500,11 +4857,167 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
+    <row r="148" spans="1:8">
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154" s="1"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" s="1"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159" s="1"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160" s="1"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" s="1"/>
+      <c r="B161" s="2"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162" s="1"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A111:G111"/>
-    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="A126:G126"/>
+    <mergeCell ref="F128:H128"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -4512,16 +5025,10 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A112:H112"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A90:H90"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A104:H104"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
25 maret edit laporan kegiatan
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari 2021 - Desember 2022_Debi Tomika.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C75A804-6A7D-458A-98F2-98C16A72DCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E452B1-9F84-4DC8-9B26-BB507D856DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1270,12 +1270,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1290,6 +1284,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:V162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1596,16 +1596,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1"/>
@@ -1824,25 +1824,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1850,13 +1850,13 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1888,16 +1888,16 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
@@ -1927,16 +1927,16 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
@@ -1993,16 +1993,16 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
@@ -2356,16 +2356,16 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="26"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="24"/>
     </row>
     <row r="42" spans="1:8" ht="42.75">
       <c r="A42" s="7">
@@ -4194,16 +4194,16 @@
       <c r="V108" s="15"/>
     </row>
     <row r="109" spans="1:22" ht="15" customHeight="1">
-      <c r="A109" s="24" t="s">
+      <c r="A109" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
-      <c r="H109" s="26"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="24"/>
     </row>
     <row r="110" spans="1:22" ht="42.75">
       <c r="A110" s="7">
@@ -4254,22 +4254,22 @@
       <c r="G111" s="11">
         <v>1</v>
       </c>
-      <c r="H111" s="12">
+      <c r="H111" s="16">
         <f>F111*G111</f>
         <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="112" spans="1:22">
-      <c r="A112" s="24" t="s">
+      <c r="A112" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B112" s="25"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
-      <c r="G112" s="25"/>
-      <c r="H112" s="26"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="24"/>
     </row>
     <row r="113" spans="1:8" ht="57">
       <c r="A113" s="7">
@@ -4623,15 +4623,15 @@
       </c>
     </row>
     <row r="126" spans="1:8">
-      <c r="A126" s="21" t="s">
+      <c r="A126" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B126" s="21"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="21"/>
-      <c r="E126" s="21"/>
-      <c r="F126" s="21"/>
-      <c r="G126" s="21"/>
+      <c r="B126" s="26"/>
+      <c r="C126" s="26"/>
+      <c r="D126" s="26"/>
+      <c r="E126" s="26"/>
+      <c r="F126" s="26"/>
+      <c r="G126" s="26"/>
       <c r="H126" s="6">
         <f>SUM(H23:H125)</f>
         <v>75.744999999999962</v>
@@ -4655,11 +4655,11 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="22" t="s">
+      <c r="F128" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="G128" s="22"/>
-      <c r="H128" s="22"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="1"/>
@@ -4667,11 +4667,11 @@
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="22" t="s">
+      <c r="F129" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G129" s="22"/>
-      <c r="H129" s="22"/>
+      <c r="G129" s="20"/>
+      <c r="H129" s="20"/>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" s="1"/>
@@ -4719,11 +4719,11 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="22" t="s">
+      <c r="F134" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="G134" s="22"/>
-      <c r="H134" s="22"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="20"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="1"/>
@@ -4731,11 +4731,11 @@
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
-      <c r="F135" s="22" t="s">
+      <c r="F135" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G135" s="22"/>
-      <c r="H135" s="22"/>
+      <c r="G135" s="20"/>
+      <c r="H135" s="20"/>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" s="1"/>
@@ -5009,12 +5009,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A126:G126"/>
     <mergeCell ref="F128:H128"/>
@@ -5029,6 +5023,12 @@
     <mergeCell ref="A112:H112"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A104:H104"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>